<commit_message>
fixed a few formulas in ETA calc
</commit_message>
<xml_diff>
--- a/NAV Log Calculator - Flight Planner - E6B-like.xlsx
+++ b/NAV Log Calculator - Flight Planner - E6B-like.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/194e8d034589e5e8/Aviation/NAV/Aviation-Navigation-Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="792" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECBF414D-D571-4244-B48B-932AC3C69678}"/>
+  <xr:revisionPtr revIDLastSave="808" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1D093F-5A4E-45D7-9DF3-5CCA7808E567}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="2" xr2:uid="{81AC26DA-A476-4998-AAF9-3938C858D589}"/>
   </bookViews>
@@ -1843,6 +1843,153 @@
     <xf numFmtId="0" fontId="45" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1866,13 +2013,7 @@
     <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1908,145 +2049,20 @@
     <xf numFmtId="0" fontId="31" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2077,10 +2093,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2108,18 +2120,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7823,7 +7823,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9 H3:I4"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7839,144 +7839,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="113">
+      <c r="B1" s="126">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="127"/>
+      <c r="E1" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="95">
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="140">
         <v>38</v>
       </c>
-      <c r="I1" s="104"/>
+      <c r="I1" s="147"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="107" t="s">
+      <c r="N1" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="108"/>
-      <c r="P1" s="95">
+      <c r="O1" s="151"/>
+      <c r="P1" s="140">
         <v>3500</v>
       </c>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="93" t="s">
+      <c r="Q1" s="140"/>
+      <c r="R1" s="138" t="s">
         <v>70</v>
       </c>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="116"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="105"/>
+      <c r="A2" s="125"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="129"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="148"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="94"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="139"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="95">
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="140">
         <v>6.5</v>
       </c>
-      <c r="I3" s="104"/>
+      <c r="I3" s="147"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="107" t="s">
+      <c r="N3" s="150" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="95">
+      <c r="O3" s="151"/>
+      <c r="P3" s="140">
         <v>215</v>
       </c>
-      <c r="Q3" s="97" t="s">
+      <c r="Q3" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="95">
+      <c r="R3" s="140">
         <v>17</v>
       </c>
-      <c r="S3" s="93" t="s">
+      <c r="S3" s="138" t="s">
         <v>71</v>
       </c>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="E4" s="102"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="105"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="98"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="99"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="148"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="155"/>
+      <c r="P4" s="141"/>
+      <c r="Q4" s="143"/>
+      <c r="R4" s="141"/>
+      <c r="S4" s="144"/>
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="135"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="128"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="135"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="129" t="s">
+      <c r="C7" s="132"/>
+      <c r="D7" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="130"/>
+      <c r="E7" s="137"/>
       <c r="F7" s="59" t="s">
         <v>2</v>
       </c>
@@ -8006,7 +8006,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19.7" customHeight="1">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="130" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -8066,49 +8066,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="122"/>
-      <c r="B9" s="120">
+      <c r="A9" s="115"/>
+      <c r="B9" s="118">
         <v>90</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="118">
         <v>3500</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="118">
         <v>215</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="118">
         <v>17</v>
       </c>
-      <c r="F9" s="120">
+      <c r="F9" s="118">
         <v>-10</v>
       </c>
-      <c r="G9" s="120">
+      <c r="G9" s="118">
         <v>95</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="117">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D9-B9))*(E9/G9)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I9" s="119">
+      <c r="I9" s="117">
         <f>IFERROR(ROUND(MOD(B9+H9,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J9" s="120">
+      <c r="J9" s="118">
         <v>13</v>
       </c>
-      <c r="K9" s="119">
+      <c r="K9" s="117">
         <f>IFERROR(MOD(I9+J9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L9" s="120">
+      <c r="L9" s="118">
         <v>0</v>
       </c>
       <c r="M9" s="7"/>
-      <c r="N9" s="119">
+      <c r="N9" s="117">
         <f>IFERROR(MOD(K9+L9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O9" s="120">
+      <c r="O9" s="118">
         <v>7</v>
       </c>
       <c r="P9" s="43">
@@ -8133,23 +8133,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="123" t="s">
+      <c r="A10" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="120"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="118"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="120"/>
+      <c r="N10" s="117"/>
+      <c r="O10" s="118"/>
       <c r="P10" s="53"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="54"/>
@@ -8157,49 +8157,49 @@
       <c r="T10" s="53"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="122"/>
-      <c r="B11" s="118">
+      <c r="A11" s="115"/>
+      <c r="B11" s="123">
         <v>90</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="123">
         <v>3500</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="123">
         <v>215</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="123">
         <v>17</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="123">
         <v>-10</v>
       </c>
-      <c r="G11" s="118">
+      <c r="G11" s="123">
         <v>95</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="121">
         <f t="shared" ref="H11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D11-B11))*(E11/G11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I11" s="117">
+      <c r="I11" s="121">
         <f>IFERROR(ROUND(MOD(B11+H11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J11" s="118">
+      <c r="J11" s="123">
         <v>13</v>
       </c>
-      <c r="K11" s="117">
+      <c r="K11" s="121">
         <f t="shared" ref="K11" si="1">IFERROR(MOD(I11+J11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L11" s="118">
+      <c r="L11" s="123">
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="117">
+      <c r="N11" s="121">
         <f>IFERROR(MOD(K11+L11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="118">
+      <c r="O11" s="123">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -8224,23 +8224,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="118"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="123"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="118"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="123"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -8248,49 +8248,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="122"/>
-      <c r="B13" s="120">
+      <c r="A13" s="115"/>
+      <c r="B13" s="118">
         <v>131</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C13" s="118">
         <v>3500</v>
       </c>
-      <c r="D13" s="120">
+      <c r="D13" s="118">
         <v>215</v>
       </c>
-      <c r="E13" s="120">
+      <c r="E13" s="118">
         <v>17</v>
       </c>
-      <c r="F13" s="120">
+      <c r="F13" s="118">
         <v>-10</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="118">
         <v>95</v>
       </c>
-      <c r="H13" s="119">
+      <c r="H13" s="117">
         <f t="shared" ref="H13" si="3">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D13-B13))*(E13/G13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I13" s="119">
+      <c r="I13" s="117">
         <f t="shared" ref="I13" si="4">IFERROR(ROUND(MOD(B13+H13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J13" s="120">
+      <c r="J13" s="118">
         <v>13</v>
       </c>
-      <c r="K13" s="119">
+      <c r="K13" s="117">
         <f t="shared" ref="K13" si="5">IFERROR(MOD(I13+J13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L13" s="120">
+      <c r="L13" s="118">
         <v>2</v>
       </c>
       <c r="M13" s="7"/>
-      <c r="N13" s="119">
+      <c r="N13" s="117">
         <f>IFERROR(MOD(K13+L13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="120">
+      <c r="O13" s="118">
         <v>11</v>
       </c>
       <c r="P13" s="43">
@@ -8315,23 +8315,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="123" t="s">
+      <c r="A14" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="120"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="117"/>
+      <c r="L14" s="118"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="120"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="118"/>
       <c r="P14" s="53"/>
       <c r="Q14" s="53"/>
       <c r="R14" s="54"/>
@@ -8339,49 +8339,49 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="122"/>
-      <c r="B15" s="131">
+      <c r="A15" s="115"/>
+      <c r="B15" s="116">
         <v>131</v>
       </c>
-      <c r="C15" s="131">
+      <c r="C15" s="116">
         <v>3500</v>
       </c>
-      <c r="D15" s="131">
+      <c r="D15" s="116">
         <v>215</v>
       </c>
-      <c r="E15" s="131">
+      <c r="E15" s="116">
         <v>17</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="116">
         <v>-10</v>
       </c>
-      <c r="G15" s="131">
+      <c r="G15" s="116">
         <v>95</v>
       </c>
-      <c r="H15" s="117">
+      <c r="H15" s="121">
         <f t="shared" ref="H15" si="7">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D15-B15))*(E15/G15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I15" s="117">
+      <c r="I15" s="121">
         <f t="shared" ref="I15" si="8">IFERROR(ROUND(MOD(B15+H15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J15" s="118">
+      <c r="J15" s="123">
         <v>13</v>
       </c>
-      <c r="K15" s="117">
+      <c r="K15" s="121">
         <f t="shared" ref="K15" si="9">IFERROR(MOD(I15+J15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L15" s="118">
+      <c r="L15" s="123">
         <v>2</v>
       </c>
       <c r="M15" s="7"/>
-      <c r="N15" s="117">
+      <c r="N15" s="121">
         <f>IFERROR(MOD(K15+L15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="118">
+      <c r="O15" s="123">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -8406,23 +8406,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="123" t="s">
+      <c r="A16" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="117"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="118"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="123"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="123"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="118"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="123"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -8430,49 +8430,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="122"/>
-      <c r="B17" s="120">
+      <c r="A17" s="115"/>
+      <c r="B17" s="118">
         <v>131</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="118">
         <v>3500</v>
       </c>
-      <c r="D17" s="120">
+      <c r="D17" s="118">
         <v>215</v>
       </c>
-      <c r="E17" s="120">
+      <c r="E17" s="118">
         <v>17</v>
       </c>
-      <c r="F17" s="120">
+      <c r="F17" s="118">
         <v>-10</v>
       </c>
-      <c r="G17" s="120">
+      <c r="G17" s="118">
         <v>95</v>
       </c>
-      <c r="H17" s="119">
+      <c r="H17" s="117">
         <f t="shared" ref="H17" si="11">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D17-B17))*(E17/G17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I17" s="119">
+      <c r="I17" s="117">
         <f t="shared" ref="I17" si="12">IFERROR(ROUND(MOD(B17+H17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J17" s="120">
+      <c r="J17" s="118">
         <v>13</v>
       </c>
-      <c r="K17" s="119">
+      <c r="K17" s="117">
         <f t="shared" ref="K17" si="13">IFERROR(MOD(I17+J17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L17" s="120">
+      <c r="L17" s="118">
         <v>2</v>
       </c>
       <c r="M17" s="7"/>
-      <c r="N17" s="119">
+      <c r="N17" s="117">
         <f>IFERROR(MOD(K17+L17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="120">
+      <c r="O17" s="118">
         <v>10</v>
       </c>
       <c r="P17" s="43">
@@ -8497,23 +8497,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="123" t="s">
+      <c r="A18" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="120"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="117"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="117"/>
+      <c r="L18" s="118"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="119"/>
-      <c r="O18" s="120"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="118"/>
       <c r="P18" s="53"/>
       <c r="Q18" s="53"/>
       <c r="R18" s="54"/>
@@ -8521,49 +8521,49 @@
       <c r="T18" s="53"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="122"/>
-      <c r="B19" s="131">
+      <c r="A19" s="115"/>
+      <c r="B19" s="116">
         <v>131</v>
       </c>
-      <c r="C19" s="131">
+      <c r="C19" s="116">
         <v>3500</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="116">
         <v>215</v>
       </c>
-      <c r="E19" s="131">
+      <c r="E19" s="116">
         <v>17</v>
       </c>
-      <c r="F19" s="131">
+      <c r="F19" s="116">
         <v>-10</v>
       </c>
-      <c r="G19" s="131">
+      <c r="G19" s="116">
         <v>95</v>
       </c>
-      <c r="H19" s="117">
+      <c r="H19" s="121">
         <f t="shared" ref="H19" si="15">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D19-B19))*(E19/G19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I19" s="117">
+      <c r="I19" s="121">
         <f t="shared" ref="I19" si="16">IFERROR(ROUND(MOD(B19+H19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J19" s="118">
+      <c r="J19" s="123">
         <v>13</v>
       </c>
-      <c r="K19" s="117">
+      <c r="K19" s="121">
         <f t="shared" ref="K19" si="17">IFERROR(MOD(I19+J19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L19" s="118">
+      <c r="L19" s="123">
         <v>2</v>
       </c>
       <c r="M19" s="7"/>
-      <c r="N19" s="117">
+      <c r="N19" s="121">
         <f>IFERROR(MOD(K19+L19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="118">
+      <c r="O19" s="123">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -8588,23 +8588,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="123" t="s">
+      <c r="A20" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="118"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="123"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="123"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="118"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="123"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -8612,33 +8612,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="122"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="119" t="str">
+      <c r="A21" s="115"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="117" t="str">
         <f t="shared" ref="H21" si="19">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D21-B21))*(E21/G21)))),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="119" t="str">
+      <c r="I21" s="117" t="str">
         <f t="shared" ref="I21" si="20">IFERROR(ROUND(MOD(B21+H21,360),0),"")</f>
         <v/>
       </c>
-      <c r="J21" s="120"/>
-      <c r="K21" s="119" t="str">
+      <c r="J21" s="118"/>
+      <c r="K21" s="117" t="str">
         <f t="shared" ref="K21" si="21">IFERROR(MOD(I21+J21,360),"")</f>
         <v/>
       </c>
-      <c r="L21" s="120"/>
+      <c r="L21" s="118"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="119" t="str">
+      <c r="N21" s="117" t="str">
         <f>IFERROR(MOD(K21+L21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="120"/>
+      <c r="O21" s="118"/>
       <c r="P21" s="43" t="str">
         <f>IFERROR(SQRT(G21^2+E21^2-2*G21*E21*COS(RADIANS(D21-B21-H21))),"")</f>
         <v/>
@@ -8661,21 +8661,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="123"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="119"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="119"/>
-      <c r="L22" s="120"/>
+      <c r="A22" s="114"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="118"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="119"/>
-      <c r="O22" s="120"/>
+      <c r="N22" s="117"/>
+      <c r="O22" s="118"/>
       <c r="P22" s="53"/>
       <c r="Q22" s="53"/>
       <c r="R22" s="54"/>
@@ -8683,33 +8683,33 @@
       <c r="T22" s="53"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="122"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="117" t="str">
+      <c r="A23" s="115"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="121" t="str">
         <f t="shared" ref="H23" si="23">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D23-B23))*(E23/G23)))),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="117" t="str">
+      <c r="I23" s="121" t="str">
         <f t="shared" ref="I23" si="24">IFERROR(ROUND(MOD(B23+H23,360),0),"")</f>
         <v/>
       </c>
-      <c r="J23" s="118"/>
-      <c r="K23" s="119" t="str">
+      <c r="J23" s="123"/>
+      <c r="K23" s="117" t="str">
         <f t="shared" ref="K23" si="25">IFERROR(MOD(I23+J23,360),"")</f>
         <v/>
       </c>
-      <c r="L23" s="118"/>
+      <c r="L23" s="123"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="119" t="str">
+      <c r="N23" s="117" t="str">
         <f>IFERROR(MOD(K23+L23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="118"/>
+      <c r="O23" s="123"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(G23^2+E23^2-2*G23*E23*COS(RADIANS(D23-B23-H23))),"")</f>
         <v/>
@@ -8732,21 +8732,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="123"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="131"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="119"/>
-      <c r="L24" s="118"/>
+      <c r="A24" s="114"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="123"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="123"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="119"/>
-      <c r="O24" s="118"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="123"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -8754,33 +8754,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="155"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="119" t="str">
+      <c r="A25" s="119"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="117" t="str">
         <f t="shared" ref="H25" si="27">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D25-B25))*(E25/G25)))),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="119" t="str">
+      <c r="I25" s="117" t="str">
         <f t="shared" ref="I25" si="28">IFERROR(ROUND(MOD(B25+H25,360),0),"")</f>
         <v/>
       </c>
-      <c r="J25" s="120"/>
-      <c r="K25" s="119" t="str">
+      <c r="J25" s="118"/>
+      <c r="K25" s="117" t="str">
         <f t="shared" ref="K25" si="29">IFERROR(MOD(I25+J25,360),"")</f>
         <v/>
       </c>
-      <c r="L25" s="120"/>
+      <c r="L25" s="118"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="119" t="str">
+      <c r="N25" s="117" t="str">
         <f>IFERROR(MOD(K25+L25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="120"/>
+      <c r="O25" s="118"/>
       <c r="P25" s="43" t="str">
         <f>IFERROR(SQRT(G25^2+E25^2-2*G25*E25*COS(RADIANS(D25-B25-H25))),"")</f>
         <v/>
@@ -8806,20 +8806,20 @@
       <c r="A26" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="132"/>
-      <c r="K26" s="133"/>
-      <c r="L26" s="132"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="120"/>
+      <c r="G26" s="120"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="120"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="120"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="132"/>
+      <c r="N26" s="117"/>
+      <c r="O26" s="120"/>
       <c r="P26" s="53"/>
       <c r="Q26" s="55"/>
       <c r="R26" s="56"/>
@@ -8827,130 +8827,256 @@
       <c r="T26" s="53"/>
     </row>
     <row r="27" spans="1:20" ht="15" customHeight="1">
-      <c r="A27" s="149" t="s">
+      <c r="A27" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="150"/>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="150"/>
-      <c r="K27" s="150"/>
-      <c r="L27" s="151"/>
-      <c r="O27" s="143">
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="110"/>
+      <c r="O27" s="102">
         <f>SUM(O9:O26)</f>
         <v>55</v>
       </c>
-      <c r="Q27" s="145">
+      <c r="Q27" s="104">
         <f>SUM(Q9:Q26)</f>
         <v>35</v>
       </c>
-      <c r="R27" s="147">
+      <c r="R27" s="106">
         <f>MAX(R9:R26)</f>
         <v>0.60763888888888895</v>
       </c>
-      <c r="S27" s="145">
+      <c r="S27" s="104">
         <f>SUM(S9:S26)</f>
         <v>3.8</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="152"/>
-      <c r="B28" s="153"/>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="153"/>
-      <c r="J28" s="153"/>
-      <c r="K28" s="153"/>
-      <c r="L28" s="154"/>
-      <c r="O28" s="144"/>
-      <c r="Q28" s="146"/>
-      <c r="R28" s="148"/>
-      <c r="S28" s="146"/>
+      <c r="A28" s="111"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="112"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="112"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="113"/>
+      <c r="O28" s="103"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="105"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="135"/>
-      <c r="C29" s="135"/>
-      <c r="D29" s="135"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
-      <c r="G29" s="135"/>
-      <c r="H29" s="135"/>
-      <c r="I29" s="135"/>
-      <c r="J29" s="135"/>
-      <c r="K29" s="135"/>
-      <c r="L29" s="136"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="137"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="138"/>
-      <c r="J30" s="138"/>
-      <c r="K30" s="138"/>
-      <c r="L30" s="139"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="97"/>
+      <c r="J30" s="97"/>
+      <c r="K30" s="97"/>
+      <c r="L30" s="98"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="137"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="138"/>
-      <c r="J31" s="138"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="139"/>
+      <c r="A31" s="96"/>
+      <c r="B31" s="97"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="97"/>
+      <c r="J31" s="97"/>
+      <c r="K31" s="97"/>
+      <c r="L31" s="98"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="137"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="138"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="138"/>
-      <c r="J32" s="138"/>
-      <c r="K32" s="138"/>
-      <c r="L32" s="139"/>
+      <c r="A32" s="96"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="98"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="140"/>
-      <c r="B33" s="141"/>
-      <c r="C33" s="141"/>
-      <c r="D33" s="141"/>
-      <c r="E33" s="141"/>
-      <c r="F33" s="141"/>
-      <c r="G33" s="141"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
-      <c r="J33" s="141"/>
-      <c r="K33" s="141"/>
-      <c r="L33" s="142"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="101"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="150">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E1:G2"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="A29:L33"/>
     <mergeCell ref="O27:O28"/>
     <mergeCell ref="Q27:Q28"/>
@@ -8975,132 +9101,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E1:G2"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="N3:O4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
@@ -9114,7 +9114,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="M12" sqref="M12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9133,134 +9133,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="160">
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="165">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E1" s="161"/>
+      <c r="E1" s="166"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="165" t="s">
+      <c r="G1" s="169" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="164">
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="160">
         <v>38</v>
       </c>
-      <c r="K1" s="164"/>
+      <c r="K1" s="160"/>
       <c r="L1" s="24"/>
-      <c r="M1" s="166" t="s">
+      <c r="M1" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="168">
+      <c r="N1" s="172">
         <v>3500</v>
       </c>
-      <c r="O1" s="168"/>
-      <c r="P1" s="174" t="s">
+      <c r="O1" s="172"/>
+      <c r="P1" s="156" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="158"/>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="168"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
       <c r="L2" s="24"/>
-      <c r="M2" s="167"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="175"/>
+      <c r="M2" s="171"/>
+      <c r="N2" s="160"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="157"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
-      <c r="G3" s="165" t="s">
+      <c r="G3" s="169" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
-      <c r="J3" s="164">
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="160">
         <v>6.5</v>
       </c>
-      <c r="K3" s="164"/>
+      <c r="K3" s="160"/>
       <c r="L3" s="25"/>
-      <c r="M3" s="169" t="s">
+      <c r="M3" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="164">
+      <c r="N3" s="160">
         <v>215</v>
       </c>
-      <c r="O3" s="164"/>
-      <c r="P3" s="176" t="s">
+      <c r="O3" s="160"/>
+      <c r="P3" s="158" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="164">
+      <c r="Q3" s="160">
         <v>17</v>
       </c>
-      <c r="R3" s="164"/>
-      <c r="S3" s="174" t="s">
+      <c r="R3" s="160"/>
+      <c r="S3" s="156" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="164"/>
-      <c r="K4" s="164"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="169"/>
+      <c r="I4" s="169"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
       <c r="L4" s="25"/>
-      <c r="M4" s="170"/>
-      <c r="N4" s="171"/>
-      <c r="O4" s="171"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="164"/>
-      <c r="R4" s="164"/>
-      <c r="S4" s="175"/>
+      <c r="M4" s="174"/>
+      <c r="N4" s="175"/>
+      <c r="O4" s="175"/>
+      <c r="P4" s="159"/>
+      <c r="Q4" s="160"/>
+      <c r="R4" s="160"/>
+      <c r="S4" s="157"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1">
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="128"/>
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="135"/>
       <c r="L6" s="26"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="128"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="135"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="172" t="s">
+      <c r="C7" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="173"/>
+      <c r="D7" s="177"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -9323,7 +9323,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="28"/>
-      <c r="M8" s="121" t="s">
+      <c r="M8" s="130" t="s">
         <v>10</v>
       </c>
       <c r="N8" s="32" t="s">
@@ -9349,49 +9349,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="120">
+      <c r="A9" s="118">
         <v>90</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="118">
         <v>3500</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="118">
         <v>170</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="118">
         <v>17</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="118">
         <v>-10</v>
       </c>
-      <c r="F9" s="120">
+      <c r="F9" s="118">
         <v>95</v>
       </c>
-      <c r="G9" s="119">
+      <c r="G9" s="117">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C9-A9))*(D9/F9)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="117">
         <f>IFERROR(ROUND(MOD(A9+G9,360),0),"")</f>
         <v>100</v>
       </c>
-      <c r="I9" s="120">
+      <c r="I9" s="118">
         <v>13</v>
       </c>
-      <c r="J9" s="119">
+      <c r="J9" s="117">
         <f>IFERROR(MOD(H9+I9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="K9" s="120">
+      <c r="K9" s="118">
         <v>0</v>
       </c>
       <c r="L9" s="29"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="119">
+      <c r="M9" s="115"/>
+      <c r="N9" s="117">
         <f>IFERROR(MOD(J9+K9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="O9" s="120">
+      <c r="O9" s="118">
         <v>7</v>
       </c>
       <c r="P9" s="42">
@@ -9416,23 +9416,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="120"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="120"/>
+      <c r="A10" s="118"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="118"/>
       <c r="L10" s="29"/>
-      <c r="M10" s="123" t="s">
+      <c r="M10" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="119"/>
-      <c r="O10" s="120"/>
+      <c r="N10" s="117"/>
+      <c r="O10" s="118"/>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="45"/>
@@ -9440,49 +9440,49 @@
       <c r="T10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="118">
+      <c r="A11" s="123">
         <v>90</v>
       </c>
-      <c r="B11" s="118">
+      <c r="B11" s="123">
         <v>3500</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="123">
         <v>215</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="123">
         <v>17</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="123">
         <v>-10</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="123">
         <v>95</v>
       </c>
-      <c r="G11" s="117">
+      <c r="G11" s="121">
         <f t="shared" ref="G11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C11-A11))*(D11/F11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="121">
         <f t="shared" ref="H11" si="1">IFERROR(ROUND(MOD(A11+G11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="I11" s="118">
+      <c r="I11" s="123">
         <v>13</v>
       </c>
-      <c r="J11" s="117">
+      <c r="J11" s="121">
         <f t="shared" ref="J11" si="2">IFERROR(MOD(H11+I11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="K11" s="118">
+      <c r="K11" s="123">
         <v>0</v>
       </c>
       <c r="L11" s="29"/>
-      <c r="M11" s="122"/>
-      <c r="N11" s="117">
+      <c r="M11" s="115"/>
+      <c r="N11" s="121">
         <f>IFERROR(MOD(J11+K11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="118">
+      <c r="O11" s="123">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -9507,23 +9507,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="118"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="118"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="123"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="123" t="s">
+      <c r="M12" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="117"/>
-      <c r="O12" s="118"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="123"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -9531,49 +9531,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="120">
+      <c r="A13" s="118">
         <v>131</v>
       </c>
-      <c r="B13" s="120">
+      <c r="B13" s="118">
         <v>3500</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C13" s="118">
         <v>215</v>
       </c>
-      <c r="D13" s="120">
+      <c r="D13" s="118">
         <v>17</v>
       </c>
-      <c r="E13" s="120">
+      <c r="E13" s="118">
         <v>-10</v>
       </c>
-      <c r="F13" s="120">
+      <c r="F13" s="118">
         <v>95</v>
       </c>
-      <c r="G13" s="119">
+      <c r="G13" s="117">
         <f t="shared" ref="G13" si="4">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C13-A13))*(D13/F13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H13" s="119">
+      <c r="H13" s="117">
         <f t="shared" ref="H13" si="5">IFERROR(ROUND(MOD(A13+G13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I13" s="120">
+      <c r="I13" s="118">
         <v>13</v>
       </c>
-      <c r="J13" s="119">
+      <c r="J13" s="117">
         <f t="shared" ref="J13" si="6">IFERROR(MOD(H13+I13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K13" s="120">
+      <c r="K13" s="118">
         <v>2</v>
       </c>
       <c r="L13" s="29"/>
-      <c r="M13" s="122"/>
-      <c r="N13" s="119">
+      <c r="M13" s="115"/>
+      <c r="N13" s="117">
         <f>IFERROR(MOD(J13+K13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="120">
+      <c r="O13" s="118">
         <v>11</v>
       </c>
       <c r="P13" s="42">
@@ -9598,23 +9598,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="120"/>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="120"/>
+      <c r="A14" s="118"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="117"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="117"/>
+      <c r="K14" s="118"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="123" t="s">
+      <c r="M14" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="119"/>
-      <c r="O14" s="120"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="118"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
       <c r="R14" s="45"/>
@@ -9622,49 +9622,49 @@
       <c r="T14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="131">
+      <c r="A15" s="116">
         <v>131</v>
       </c>
-      <c r="B15" s="131">
+      <c r="B15" s="116">
         <v>3500</v>
       </c>
-      <c r="C15" s="131">
+      <c r="C15" s="116">
         <v>215</v>
       </c>
-      <c r="D15" s="131">
+      <c r="D15" s="116">
         <v>17</v>
       </c>
-      <c r="E15" s="131">
+      <c r="E15" s="116">
         <v>-10</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="116">
         <v>95</v>
       </c>
-      <c r="G15" s="117">
+      <c r="G15" s="121">
         <f t="shared" ref="G15" si="8">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C15-A15))*(D15/F15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H15" s="117">
+      <c r="H15" s="121">
         <f t="shared" ref="H15" si="9">IFERROR(ROUND(MOD(A15+G15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I15" s="118">
+      <c r="I15" s="123">
         <v>13</v>
       </c>
-      <c r="J15" s="117">
+      <c r="J15" s="121">
         <f t="shared" ref="J15" si="10">IFERROR(MOD(H15+I15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K15" s="118">
+      <c r="K15" s="123">
         <v>2</v>
       </c>
       <c r="L15" s="29"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="117">
+      <c r="M15" s="115"/>
+      <c r="N15" s="121">
         <f>IFERROR(MOD(J15+K15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="118">
+      <c r="O15" s="123">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -9676,7 +9676,7 @@
         <v>5</v>
       </c>
       <c r="R15" s="47">
-        <f>IFERROR(Departure_Time+SUM($Q$9:Q16)/60/24,"")</f>
+        <f>IF(Q15&lt;&gt;"",IFERROR(Departure_Time+SUM($Q$9:Q16)/60/24,""),"")</f>
         <v>0.65069444444444435</v>
       </c>
       <c r="S15" s="46">
@@ -9689,23 +9689,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="131"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="118"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="123"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="123"/>
       <c r="L16" s="29"/>
-      <c r="M16" s="123" t="s">
+      <c r="M16" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="117"/>
-      <c r="O16" s="118"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="123"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -9713,49 +9713,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="120">
+      <c r="A17" s="118">
         <v>131</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="118">
         <v>3500</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="118">
         <v>215</v>
       </c>
-      <c r="D17" s="120">
+      <c r="D17" s="118">
         <v>17</v>
       </c>
-      <c r="E17" s="120">
+      <c r="E17" s="118">
         <v>-10</v>
       </c>
-      <c r="F17" s="120">
+      <c r="F17" s="118">
         <v>95</v>
       </c>
-      <c r="G17" s="119">
+      <c r="G17" s="117">
         <f t="shared" ref="G17" si="12">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C17-A17))*(D17/F17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H17" s="119">
+      <c r="H17" s="117">
         <f t="shared" ref="H17" si="13">IFERROR(ROUND(MOD(A17+G17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I17" s="120">
+      <c r="I17" s="118">
         <v>13</v>
       </c>
-      <c r="J17" s="119">
+      <c r="J17" s="117">
         <f t="shared" ref="J17" si="14">IFERROR(MOD(H17+I17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K17" s="120">
+      <c r="K17" s="118">
         <v>2</v>
       </c>
       <c r="L17" s="29"/>
-      <c r="M17" s="122"/>
-      <c r="N17" s="119">
+      <c r="M17" s="115"/>
+      <c r="N17" s="117">
         <f>IFERROR(MOD(J17+K17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="120">
+      <c r="O17" s="118">
         <v>10</v>
       </c>
       <c r="P17" s="42">
@@ -9780,23 +9780,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="120"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
+      <c r="A18" s="118"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="117"/>
+      <c r="K18" s="118"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="123" t="s">
+      <c r="M18" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="119"/>
-      <c r="O18" s="120"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="118"/>
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
       <c r="R18" s="45"/>
@@ -9804,49 +9804,49 @@
       <c r="T18" s="44"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="131">
+      <c r="A19" s="116">
         <v>131</v>
       </c>
-      <c r="B19" s="131">
+      <c r="B19" s="116">
         <v>3500</v>
       </c>
-      <c r="C19" s="131">
+      <c r="C19" s="116">
         <v>215</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="116">
         <v>17</v>
       </c>
-      <c r="E19" s="131">
+      <c r="E19" s="116">
         <v>-10</v>
       </c>
-      <c r="F19" s="131">
+      <c r="F19" s="116">
         <v>95</v>
       </c>
-      <c r="G19" s="117">
+      <c r="G19" s="121">
         <f t="shared" ref="G19" si="16">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C19-A19))*(D19/F19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H19" s="117">
+      <c r="H19" s="121">
         <f t="shared" ref="H19" si="17">IFERROR(ROUND(MOD(A19+G19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I19" s="118">
+      <c r="I19" s="123">
         <v>13</v>
       </c>
-      <c r="J19" s="117">
+      <c r="J19" s="121">
         <f t="shared" ref="J19" si="18">IFERROR(MOD(H19+I19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K19" s="118">
+      <c r="K19" s="123">
         <v>2</v>
       </c>
       <c r="L19" s="29"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="117">
+      <c r="M19" s="115"/>
+      <c r="N19" s="121">
         <f>IFERROR(MOD(J19+K19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="118">
+      <c r="O19" s="123">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -9871,23 +9871,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="131"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="118"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="123"/>
+      <c r="J20" s="121"/>
+      <c r="K20" s="123"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="123" t="s">
+      <c r="M20" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="N20" s="117"/>
-      <c r="O20" s="118"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="123"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -9895,33 +9895,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="120"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="119" t="str">
+      <c r="A21" s="118"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="117" t="str">
         <f t="shared" ref="G21" si="20">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C21-A21))*(D21/F21)))),0),"")</f>
         <v/>
       </c>
-      <c r="H21" s="119" t="str">
+      <c r="H21" s="117" t="str">
         <f t="shared" ref="H21" si="21">IFERROR(ROUND(MOD(A21+G21,360),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="120"/>
-      <c r="J21" s="119" t="str">
+      <c r="I21" s="118"/>
+      <c r="J21" s="117" t="str">
         <f t="shared" ref="J21" si="22">IFERROR(MOD(H21+I21,360),"")</f>
         <v/>
       </c>
-      <c r="K21" s="120"/>
+      <c r="K21" s="118"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="119" t="str">
+      <c r="M21" s="115"/>
+      <c r="N21" s="117" t="str">
         <f>IFERROR(MOD(J21+K21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="120"/>
+      <c r="O21" s="118"/>
       <c r="P21" s="42" t="str">
         <f>IFERROR(SQRT(F21^2+D21^2-2*F21*D21*COS(RADIANS(C21-A21-G21))),"")</f>
         <v/>
@@ -9944,21 +9944,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="119"/>
-      <c r="K22" s="120"/>
+      <c r="A22" s="118"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="118"/>
       <c r="L22" s="29"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="119"/>
-      <c r="O22" s="120"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="117"/>
+      <c r="O22" s="118"/>
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="45"/>
@@ -9966,33 +9966,33 @@
       <c r="T22" s="44"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="131"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="117" t="str">
+      <c r="A23" s="116"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="121" t="str">
         <f t="shared" ref="G23" si="24">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C23-A23))*(D23/F23)))),0),"")</f>
         <v/>
       </c>
-      <c r="H23" s="117" t="str">
+      <c r="H23" s="121" t="str">
         <f t="shared" ref="H23" si="25">IFERROR(ROUND(MOD(A23+G23,360),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="118"/>
-      <c r="J23" s="117" t="str">
+      <c r="I23" s="123"/>
+      <c r="J23" s="121" t="str">
         <f t="shared" ref="J23" si="26">IFERROR(MOD(H23+I23,360),"")</f>
         <v/>
       </c>
-      <c r="K23" s="118"/>
+      <c r="K23" s="123"/>
       <c r="L23" s="29"/>
-      <c r="M23" s="122"/>
-      <c r="N23" s="117" t="str">
+      <c r="M23" s="115"/>
+      <c r="N23" s="121" t="str">
         <f>IFERROR(MOD(J23+K23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="118"/>
+      <c r="O23" s="123"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(F23^2+D23^2-2*F23*D23*COS(RADIANS(C23-A23-G23))),"")</f>
         <v/>
@@ -10015,21 +10015,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="131"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="118"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="123"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="123"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="118"/>
+      <c r="M24" s="114"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="123"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -10037,33 +10037,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="120"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="119" t="str">
+      <c r="A25" s="118"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="117" t="str">
         <f t="shared" ref="G25" si="28">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C25-A25))*(D25/F25)))),0),"")</f>
         <v/>
       </c>
-      <c r="H25" s="119" t="str">
+      <c r="H25" s="117" t="str">
         <f t="shared" ref="H25" si="29">IFERROR(ROUND(MOD(A25+G25,360),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="120"/>
-      <c r="J25" s="119" t="str">
+      <c r="I25" s="118"/>
+      <c r="J25" s="117" t="str">
         <f t="shared" ref="J25" si="30">IFERROR(MOD(H25+I25,360),"")</f>
         <v/>
       </c>
-      <c r="K25" s="120"/>
+      <c r="K25" s="118"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="155"/>
-      <c r="N25" s="119" t="str">
+      <c r="M25" s="119"/>
+      <c r="N25" s="117" t="str">
         <f>IFERROR(MOD(J25+K25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="120"/>
+      <c r="O25" s="118"/>
       <c r="P25" s="42" t="str">
         <f>IFERROR(SQRT(F25^2+D25^2-2*F25*D25*COS(RADIANS(C25-A25-G25))),"")</f>
         <v/>
@@ -10086,23 +10086,23 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A26" s="120"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="119"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="120"/>
+      <c r="A26" s="118"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="117"/>
+      <c r="K26" s="118"/>
       <c r="L26" s="29"/>
       <c r="M26" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N26" s="119"/>
-      <c r="O26" s="120"/>
+      <c r="N26" s="117"/>
+      <c r="O26" s="118"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
       <c r="R26" s="45"/>
@@ -10110,19 +10110,19 @@
       <c r="T26" s="44"/>
     </row>
     <row r="27" spans="1:20" ht="25.5" thickBot="1">
-      <c r="A27" s="137" t="s">
+      <c r="A27" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
-      <c r="J27" s="138"/>
-      <c r="K27" s="139"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="98"/>
       <c r="L27" s="30"/>
       <c r="M27" s="31" t="s">
         <v>67</v>
@@ -10145,23 +10145,143 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A28" s="140"/>
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="141"/>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="142"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="101"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="144">
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="A27:K28"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="O11:O12"/>
@@ -10186,126 +10306,6 @@
     <mergeCell ref="Q3:R4"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A27:K28"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="G1:I2"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:O4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -10318,7 +10318,7 @@
   <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added instructions for cross wind calculator
</commit_message>
<xml_diff>
--- a/NAV Log Calculator - Flight Planner - E6B-like.xlsx
+++ b/NAV Log Calculator - Flight Planner - E6B-like.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/194e8d034589e5e8/Aviation/NAV/Aviation-Navigation-Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="808" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1D093F-5A4E-45D7-9DF3-5CCA7808E567}"/>
+  <xr:revisionPtr revIDLastSave="843" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50546B89-F616-4239-B235-D113ADF453BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="2" xr2:uid="{81AC26DA-A476-4998-AAF9-3938C858D589}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="3" xr2:uid="{81AC26DA-A476-4998-AAF9-3938C858D589}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t>TC</t>
   </si>
@@ -603,6 +603,145 @@
   </si>
   <si>
     <t>RWY Cross wind component (Calculator)</t>
+  </si>
+  <si>
+    <t>Instructions:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fill the following:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plane Heading</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (used to calculate the WCA)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>True Air Speed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (also used to calculate the WCA)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wind Direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (used to calculate the WCA and the X/wind component)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wind Speed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (also used to calculate the WCA and the X/wind component)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Runway (2 digits)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - used to calculate the X/wind and H/wind components</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The wind makes an angle with the runway. If you treat that wind vector as the hypothenus of a regtangle triangle (this hypothenus length being the wind speed) which adjacent side is the runway, your cross-wind component will be the opposite side of that rectangle triangle - the opposite side being the side which has a 90 degrees angle with the adjacent/runway side. In other words, it's the part of the wind that blows perpendicularily to  the runway and then to the plane when it's aligned to take off. The length of the perpendicular wind component will be the cross wind speed.
+The formula to get the length (aka the force) of that opposite side of that rectangle triangle is :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SIN(angle between runway and wind) x Wind speed</t>
+    </r>
+  </si>
+  <si>
+    <t>Note about the formula used:</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1843,256 +1982,244 @@
     <xf numFmtId="0" fontId="45" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="17" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="17" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2122,6 +2249,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2145,6 +2284,58 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6992,7 +7183,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>338550</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>114736</xdr:rowOff>
+      <xdr:rowOff>102830</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -7007,7 +7198,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1300163" y="4724405"/>
+          <a:off x="1300163" y="4748217"/>
           <a:ext cx="4312856" cy="4320019"/>
           <a:chOff x="0" y="3938592"/>
           <a:chExt cx="4320000" cy="4320019"/>
@@ -7109,7 +7300,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>147638</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>78006</xdr:rowOff>
+      <xdr:rowOff>66100</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -7124,7 +7315,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3105175" y="566738"/>
+          <a:off x="3105175" y="578644"/>
           <a:ext cx="2316932" cy="2344956"/>
           <a:chOff x="4414856" y="295255"/>
           <a:chExt cx="4324746" cy="4339070"/>
@@ -7839,144 +8030,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="126">
+      <c r="B1" s="113">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="E1" s="124" t="s">
+      <c r="C1" s="114"/>
+      <c r="E1" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="140">
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="95">
         <v>38</v>
       </c>
-      <c r="I1" s="147"/>
+      <c r="I1" s="104"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="150" t="s">
+      <c r="N1" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="151"/>
-      <c r="P1" s="140">
+      <c r="O1" s="108"/>
+      <c r="P1" s="95">
         <v>3500</v>
       </c>
-      <c r="Q1" s="140"/>
-      <c r="R1" s="138" t="s">
+      <c r="Q1" s="95"/>
+      <c r="R1" s="93" t="s">
         <v>70</v>
       </c>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="125"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="129"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="148"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="116"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="105"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="153"/>
-      <c r="P2" s="149"/>
-      <c r="Q2" s="149"/>
-      <c r="R2" s="139"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="94"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="140">
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="95">
         <v>6.5</v>
       </c>
-      <c r="I3" s="147"/>
+      <c r="I3" s="104"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="150" t="s">
+      <c r="N3" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="151"/>
-      <c r="P3" s="140">
+      <c r="O3" s="108"/>
+      <c r="P3" s="95">
         <v>215</v>
       </c>
-      <c r="Q3" s="142" t="s">
+      <c r="Q3" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="140">
+      <c r="R3" s="95">
         <v>17</v>
       </c>
-      <c r="S3" s="138" t="s">
+      <c r="S3" s="93" t="s">
         <v>71</v>
       </c>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="E4" s="125"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="148"/>
-      <c r="N4" s="154"/>
-      <c r="O4" s="155"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="143"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="144"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="105"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="99"/>
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="134"/>
-      <c r="L6" s="135"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="133" t="s">
+      <c r="N6" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="134"/>
-      <c r="R6" s="134"/>
-      <c r="S6" s="134"/>
-      <c r="T6" s="135"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="127"/>
+      <c r="S6" s="127"/>
+      <c r="T6" s="128"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="132"/>
-      <c r="D7" s="136" t="s">
+      <c r="C7" s="125"/>
+      <c r="D7" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="137"/>
+      <c r="E7" s="130"/>
       <c r="F7" s="59" t="s">
         <v>2</v>
       </c>
@@ -8006,7 +8197,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19.7" customHeight="1">
-      <c r="A8" s="130" t="s">
+      <c r="A8" s="121" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -8066,49 +8257,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="115"/>
-      <c r="B9" s="118">
+      <c r="A9" s="122"/>
+      <c r="B9" s="120">
         <v>90</v>
       </c>
-      <c r="C9" s="118">
+      <c r="C9" s="120">
         <v>3500</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D9" s="120">
         <v>215</v>
       </c>
-      <c r="E9" s="118">
+      <c r="E9" s="120">
         <v>17</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="120">
         <v>-10</v>
       </c>
-      <c r="G9" s="118">
+      <c r="G9" s="120">
         <v>95</v>
       </c>
-      <c r="H9" s="117">
+      <c r="H9" s="119">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D9-B9))*(E9/G9)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="119">
         <f>IFERROR(ROUND(MOD(B9+H9,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J9" s="118">
+      <c r="J9" s="120">
         <v>13</v>
       </c>
-      <c r="K9" s="117">
+      <c r="K9" s="119">
         <f>IFERROR(MOD(I9+J9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L9" s="118">
+      <c r="L9" s="120">
         <v>0</v>
       </c>
       <c r="M9" s="7"/>
-      <c r="N9" s="117">
+      <c r="N9" s="119">
         <f>IFERROR(MOD(K9+L9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O9" s="118">
+      <c r="O9" s="120">
         <v>7</v>
       </c>
       <c r="P9" s="43">
@@ -8133,23 +8324,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
-      <c r="J10" s="118"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="118"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="120"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="118"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="120"/>
       <c r="P10" s="53"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="54"/>
@@ -8157,49 +8348,49 @@
       <c r="T10" s="53"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="115"/>
-      <c r="B11" s="123">
+      <c r="A11" s="122"/>
+      <c r="B11" s="118">
         <v>90</v>
       </c>
-      <c r="C11" s="123">
+      <c r="C11" s="118">
         <v>3500</v>
       </c>
-      <c r="D11" s="123">
+      <c r="D11" s="118">
         <v>215</v>
       </c>
-      <c r="E11" s="123">
+      <c r="E11" s="118">
         <v>17</v>
       </c>
-      <c r="F11" s="123">
+      <c r="F11" s="118">
         <v>-10</v>
       </c>
-      <c r="G11" s="123">
+      <c r="G11" s="118">
         <v>95</v>
       </c>
-      <c r="H11" s="121">
+      <c r="H11" s="117">
         <f t="shared" ref="H11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D11-B11))*(E11/G11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I11" s="121">
+      <c r="I11" s="117">
         <f>IFERROR(ROUND(MOD(B11+H11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J11" s="123">
+      <c r="J11" s="118">
         <v>13</v>
       </c>
-      <c r="K11" s="121">
+      <c r="K11" s="117">
         <f t="shared" ref="K11" si="1">IFERROR(MOD(I11+J11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L11" s="123">
+      <c r="L11" s="118">
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="121">
+      <c r="N11" s="117">
         <f>IFERROR(MOD(K11+L11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="123">
+      <c r="O11" s="118">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -8224,23 +8415,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="121"/>
-      <c r="I12" s="121"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="123"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="118"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="121"/>
-      <c r="O12" s="123"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="118"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -8248,49 +8439,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="115"/>
-      <c r="B13" s="118">
+      <c r="A13" s="122"/>
+      <c r="B13" s="120">
         <v>131</v>
       </c>
-      <c r="C13" s="118">
+      <c r="C13" s="120">
         <v>3500</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D13" s="120">
         <v>215</v>
       </c>
-      <c r="E13" s="118">
+      <c r="E13" s="120">
         <v>17</v>
       </c>
-      <c r="F13" s="118">
+      <c r="F13" s="120">
         <v>-10</v>
       </c>
-      <c r="G13" s="118">
+      <c r="G13" s="120">
         <v>95</v>
       </c>
-      <c r="H13" s="117">
+      <c r="H13" s="119">
         <f t="shared" ref="H13" si="3">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D13-B13))*(E13/G13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I13" s="117">
+      <c r="I13" s="119">
         <f t="shared" ref="I13" si="4">IFERROR(ROUND(MOD(B13+H13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J13" s="118">
+      <c r="J13" s="120">
         <v>13</v>
       </c>
-      <c r="K13" s="117">
+      <c r="K13" s="119">
         <f t="shared" ref="K13" si="5">IFERROR(MOD(I13+J13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L13" s="118">
+      <c r="L13" s="120">
         <v>2</v>
       </c>
       <c r="M13" s="7"/>
-      <c r="N13" s="117">
+      <c r="N13" s="119">
         <f>IFERROR(MOD(K13+L13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="118">
+      <c r="O13" s="120">
         <v>11</v>
       </c>
       <c r="P13" s="43">
@@ -8315,23 +8506,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="117"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="117"/>
-      <c r="L14" s="118"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="120"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="118"/>
+      <c r="N14" s="119"/>
+      <c r="O14" s="120"/>
       <c r="P14" s="53"/>
       <c r="Q14" s="53"/>
       <c r="R14" s="54"/>
@@ -8339,49 +8530,49 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="116">
+      <c r="A15" s="122"/>
+      <c r="B15" s="131">
         <v>131</v>
       </c>
-      <c r="C15" s="116">
+      <c r="C15" s="131">
         <v>3500</v>
       </c>
-      <c r="D15" s="116">
+      <c r="D15" s="131">
         <v>215</v>
       </c>
-      <c r="E15" s="116">
+      <c r="E15" s="131">
         <v>17</v>
       </c>
-      <c r="F15" s="116">
+      <c r="F15" s="131">
         <v>-10</v>
       </c>
-      <c r="G15" s="116">
+      <c r="G15" s="131">
         <v>95</v>
       </c>
-      <c r="H15" s="121">
+      <c r="H15" s="117">
         <f t="shared" ref="H15" si="7">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D15-B15))*(E15/G15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I15" s="121">
+      <c r="I15" s="117">
         <f t="shared" ref="I15" si="8">IFERROR(ROUND(MOD(B15+H15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J15" s="123">
+      <c r="J15" s="118">
         <v>13</v>
       </c>
-      <c r="K15" s="121">
+      <c r="K15" s="117">
         <f t="shared" ref="K15" si="9">IFERROR(MOD(I15+J15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L15" s="123">
+      <c r="L15" s="118">
         <v>2</v>
       </c>
       <c r="M15" s="7"/>
-      <c r="N15" s="121">
+      <c r="N15" s="117">
         <f>IFERROR(MOD(K15+L15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="123">
+      <c r="O15" s="118">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -8406,23 +8597,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="121"/>
-      <c r="L16" s="123"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="118"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="121"/>
-      <c r="O16" s="123"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="118"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -8430,49 +8621,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="115"/>
-      <c r="B17" s="118">
+      <c r="A17" s="122"/>
+      <c r="B17" s="120">
         <v>131</v>
       </c>
-      <c r="C17" s="118">
+      <c r="C17" s="120">
         <v>3500</v>
       </c>
-      <c r="D17" s="118">
+      <c r="D17" s="120">
         <v>215</v>
       </c>
-      <c r="E17" s="118">
+      <c r="E17" s="120">
         <v>17</v>
       </c>
-      <c r="F17" s="118">
+      <c r="F17" s="120">
         <v>-10</v>
       </c>
-      <c r="G17" s="118">
+      <c r="G17" s="120">
         <v>95</v>
       </c>
-      <c r="H17" s="117">
+      <c r="H17" s="119">
         <f t="shared" ref="H17" si="11">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D17-B17))*(E17/G17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I17" s="117">
+      <c r="I17" s="119">
         <f t="shared" ref="I17" si="12">IFERROR(ROUND(MOD(B17+H17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J17" s="118">
+      <c r="J17" s="120">
         <v>13</v>
       </c>
-      <c r="K17" s="117">
+      <c r="K17" s="119">
         <f t="shared" ref="K17" si="13">IFERROR(MOD(I17+J17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L17" s="118">
+      <c r="L17" s="120">
         <v>2</v>
       </c>
       <c r="M17" s="7"/>
-      <c r="N17" s="117">
+      <c r="N17" s="119">
         <f>IFERROR(MOD(K17+L17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="118">
+      <c r="O17" s="120">
         <v>10</v>
       </c>
       <c r="P17" s="43">
@@ -8497,23 +8688,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="117"/>
-      <c r="I18" s="117"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="118"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="120"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="118"/>
+      <c r="N18" s="119"/>
+      <c r="O18" s="120"/>
       <c r="P18" s="53"/>
       <c r="Q18" s="53"/>
       <c r="R18" s="54"/>
@@ -8521,49 +8712,49 @@
       <c r="T18" s="53"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="115"/>
-      <c r="B19" s="116">
+      <c r="A19" s="122"/>
+      <c r="B19" s="131">
         <v>131</v>
       </c>
-      <c r="C19" s="116">
+      <c r="C19" s="131">
         <v>3500</v>
       </c>
-      <c r="D19" s="116">
+      <c r="D19" s="131">
         <v>215</v>
       </c>
-      <c r="E19" s="116">
+      <c r="E19" s="131">
         <v>17</v>
       </c>
-      <c r="F19" s="116">
+      <c r="F19" s="131">
         <v>-10</v>
       </c>
-      <c r="G19" s="116">
+      <c r="G19" s="131">
         <v>95</v>
       </c>
-      <c r="H19" s="121">
+      <c r="H19" s="117">
         <f t="shared" ref="H19" si="15">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D19-B19))*(E19/G19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I19" s="121">
+      <c r="I19" s="117">
         <f t="shared" ref="I19" si="16">IFERROR(ROUND(MOD(B19+H19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J19" s="123">
+      <c r="J19" s="118">
         <v>13</v>
       </c>
-      <c r="K19" s="121">
+      <c r="K19" s="117">
         <f t="shared" ref="K19" si="17">IFERROR(MOD(I19+J19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L19" s="123">
+      <c r="L19" s="118">
         <v>2</v>
       </c>
       <c r="M19" s="7"/>
-      <c r="N19" s="121">
+      <c r="N19" s="117">
         <f>IFERROR(MOD(K19+L19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="123">
+      <c r="O19" s="118">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -8588,23 +8779,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="114" t="s">
+      <c r="A20" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="123"/>
-      <c r="K20" s="121"/>
-      <c r="L20" s="123"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="117"/>
+      <c r="L20" s="118"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="121"/>
-      <c r="O20" s="123"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="118"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -8612,33 +8803,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="115"/>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="117" t="str">
+      <c r="A21" s="122"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="119" t="str">
         <f t="shared" ref="H21" si="19">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D21-B21))*(E21/G21)))),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="117" t="str">
+      <c r="I21" s="119" t="str">
         <f t="shared" ref="I21" si="20">IFERROR(ROUND(MOD(B21+H21,360),0),"")</f>
         <v/>
       </c>
-      <c r="J21" s="118"/>
-      <c r="K21" s="117" t="str">
+      <c r="J21" s="120"/>
+      <c r="K21" s="119" t="str">
         <f t="shared" ref="K21" si="21">IFERROR(MOD(I21+J21,360),"")</f>
         <v/>
       </c>
-      <c r="L21" s="118"/>
+      <c r="L21" s="120"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="117" t="str">
+      <c r="N21" s="119" t="str">
         <f>IFERROR(MOD(K21+L21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="118"/>
+      <c r="O21" s="120"/>
       <c r="P21" s="43" t="str">
         <f>IFERROR(SQRT(G21^2+E21^2-2*G21*E21*COS(RADIANS(D21-B21-H21))),"")</f>
         <v/>
@@ -8661,21 +8852,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="114"/>
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="118"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="120"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="118"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="120"/>
       <c r="P22" s="53"/>
       <c r="Q22" s="53"/>
       <c r="R22" s="54"/>
@@ -8683,33 +8874,33 @@
       <c r="T22" s="53"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="115"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="121" t="str">
+      <c r="A23" s="122"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="131"/>
+      <c r="H23" s="117" t="str">
         <f t="shared" ref="H23" si="23">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D23-B23))*(E23/G23)))),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="121" t="str">
+      <c r="I23" s="117" t="str">
         <f t="shared" ref="I23" si="24">IFERROR(ROUND(MOD(B23+H23,360),0),"")</f>
         <v/>
       </c>
-      <c r="J23" s="123"/>
-      <c r="K23" s="117" t="str">
+      <c r="J23" s="118"/>
+      <c r="K23" s="119" t="str">
         <f t="shared" ref="K23" si="25">IFERROR(MOD(I23+J23,360),"")</f>
         <v/>
       </c>
-      <c r="L23" s="123"/>
+      <c r="L23" s="118"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="117" t="str">
+      <c r="N23" s="119" t="str">
         <f>IFERROR(MOD(K23+L23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="123"/>
+      <c r="O23" s="118"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(G23^2+E23^2-2*G23*E23*COS(RADIANS(D23-B23-H23))),"")</f>
         <v/>
@@ -8732,21 +8923,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="114"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="123"/>
+      <c r="A24" s="123"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="118"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="123"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="118"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -8754,33 +8945,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="119"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="117" t="str">
+      <c r="A25" s="155"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="120"/>
+      <c r="G25" s="120"/>
+      <c r="H25" s="119" t="str">
         <f t="shared" ref="H25" si="27">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D25-B25))*(E25/G25)))),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="117" t="str">
+      <c r="I25" s="119" t="str">
         <f t="shared" ref="I25" si="28">IFERROR(ROUND(MOD(B25+H25,360),0),"")</f>
         <v/>
       </c>
-      <c r="J25" s="118"/>
-      <c r="K25" s="117" t="str">
+      <c r="J25" s="120"/>
+      <c r="K25" s="119" t="str">
         <f t="shared" ref="K25" si="29">IFERROR(MOD(I25+J25,360),"")</f>
         <v/>
       </c>
-      <c r="L25" s="118"/>
+      <c r="L25" s="120"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="117" t="str">
+      <c r="N25" s="119" t="str">
         <f>IFERROR(MOD(K25+L25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="118"/>
+      <c r="O25" s="120"/>
       <c r="P25" s="43" t="str">
         <f>IFERROR(SQRT(G25^2+E25^2-2*G25*E25*COS(RADIANS(D25-B25-H25))),"")</f>
         <v/>
@@ -8806,20 +8997,20 @@
       <c r="A26" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="120"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="122"/>
-      <c r="L26" s="120"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="132"/>
+      <c r="H26" s="133"/>
+      <c r="I26" s="133"/>
+      <c r="J26" s="132"/>
+      <c r="K26" s="133"/>
+      <c r="L26" s="132"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="117"/>
-      <c r="O26" s="120"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="132"/>
       <c r="P26" s="53"/>
       <c r="Q26" s="55"/>
       <c r="R26" s="56"/>
@@ -8827,142 +9018,244 @@
       <c r="T26" s="53"/>
     </row>
     <row r="27" spans="1:20" ht="15" customHeight="1">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="149" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="110"/>
-      <c r="O27" s="102">
+      <c r="B27" s="150"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="150"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="150"/>
+      <c r="L27" s="151"/>
+      <c r="O27" s="143">
         <f>SUM(O9:O26)</f>
         <v>55</v>
       </c>
-      <c r="Q27" s="104">
+      <c r="Q27" s="145">
         <f>SUM(Q9:Q26)</f>
         <v>35</v>
       </c>
-      <c r="R27" s="106">
+      <c r="R27" s="147">
         <f>MAX(R9:R26)</f>
         <v>0.60763888888888895</v>
       </c>
-      <c r="S27" s="104">
+      <c r="S27" s="145">
         <f>SUM(S9:S26)</f>
         <v>3.8</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="111"/>
-      <c r="B28" s="112"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="112"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="113"/>
-      <c r="O28" s="103"/>
-      <c r="Q28" s="105"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="105"/>
+      <c r="A28" s="152"/>
+      <c r="B28" s="153"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="153"/>
+      <c r="I28" s="153"/>
+      <c r="J28" s="153"/>
+      <c r="K28" s="153"/>
+      <c r="L28" s="154"/>
+      <c r="O28" s="144"/>
+      <c r="Q28" s="146"/>
+      <c r="R28" s="148"/>
+      <c r="S28" s="146"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="95"/>
+      <c r="B29" s="135"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="135"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="135"/>
+      <c r="J29" s="135"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="136"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="96"/>
-      <c r="B30" s="97"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="97"/>
-      <c r="I30" s="97"/>
-      <c r="J30" s="97"/>
-      <c r="K30" s="97"/>
-      <c r="L30" s="98"/>
+      <c r="A30" s="137"/>
+      <c r="B30" s="138"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="138"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="138"/>
+      <c r="K30" s="138"/>
+      <c r="L30" s="139"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="96"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="97"/>
-      <c r="J31" s="97"/>
-      <c r="K31" s="97"/>
-      <c r="L31" s="98"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="138"/>
+      <c r="K31" s="138"/>
+      <c r="L31" s="139"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="96"/>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="97"/>
-      <c r="L32" s="98"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="138"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="138"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="139"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="99"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="100"/>
-      <c r="K33" s="100"/>
-      <c r="L33" s="101"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="141"/>
+      <c r="C33" s="141"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141"/>
+      <c r="F33" s="141"/>
+      <c r="G33" s="141"/>
+      <c r="H33" s="141"/>
+      <c r="I33" s="141"/>
+      <c r="J33" s="141"/>
+      <c r="K33" s="141"/>
+      <c r="L33" s="142"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="150">
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E1:G2"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="A29:L33"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="Q27:Q28"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="R27:R28"/>
+    <mergeCell ref="A27:L28"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="N11:N12"/>
@@ -8987,120 +9280,18 @@
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="A29:L33"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="R27:R28"/>
-    <mergeCell ref="A27:L28"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E1:G2"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="N3:O4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
@@ -9113,8 +9304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4157655B-8A58-497F-BBC8-F24326906F8C}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:M13"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9133,134 +9324,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="165">
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="160">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E1" s="166"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="169" t="s">
+      <c r="G1" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="169"/>
-      <c r="I1" s="169"/>
-      <c r="J1" s="160">
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="164">
         <v>38</v>
       </c>
-      <c r="K1" s="160"/>
+      <c r="K1" s="164"/>
       <c r="L1" s="24"/>
-      <c r="M1" s="170" t="s">
+      <c r="M1" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="172">
+      <c r="N1" s="168">
         <v>3500</v>
       </c>
-      <c r="O1" s="172"/>
-      <c r="P1" s="156" t="s">
+      <c r="O1" s="168"/>
+      <c r="P1" s="174" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
+      <c r="A2" s="158"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="163"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
       <c r="L2" s="24"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="160"/>
-      <c r="O2" s="160"/>
-      <c r="P2" s="157"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="164"/>
+      <c r="P2" s="175"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
-      <c r="G3" s="169" t="s">
+      <c r="G3" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="160">
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
+      <c r="J3" s="164">
         <v>6.5</v>
       </c>
-      <c r="K3" s="160"/>
+      <c r="K3" s="164"/>
       <c r="L3" s="25"/>
-      <c r="M3" s="173" t="s">
+      <c r="M3" s="169" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="160">
+      <c r="N3" s="164">
         <v>215</v>
       </c>
-      <c r="O3" s="160"/>
-      <c r="P3" s="158" t="s">
+      <c r="O3" s="164"/>
+      <c r="P3" s="176" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="160">
+      <c r="Q3" s="164">
         <v>17</v>
       </c>
-      <c r="R3" s="160"/>
-      <c r="S3" s="156" t="s">
+      <c r="R3" s="164"/>
+      <c r="S3" s="174" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="G4" s="169"/>
-      <c r="H4" s="169"/>
-      <c r="I4" s="169"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
+      <c r="G4" s="165"/>
+      <c r="H4" s="165"/>
+      <c r="I4" s="165"/>
+      <c r="J4" s="164"/>
+      <c r="K4" s="164"/>
       <c r="L4" s="25"/>
-      <c r="M4" s="174"/>
-      <c r="N4" s="175"/>
-      <c r="O4" s="175"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="160"/>
-      <c r="R4" s="160"/>
-      <c r="S4" s="157"/>
+      <c r="M4" s="170"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="164"/>
+      <c r="R4" s="164"/>
+      <c r="S4" s="175"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1">
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="134"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="135"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="128"/>
       <c r="L6" s="26"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="133" t="s">
+      <c r="N6" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="134"/>
-      <c r="R6" s="134"/>
-      <c r="S6" s="134"/>
-      <c r="T6" s="135"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="127"/>
+      <c r="S6" s="127"/>
+      <c r="T6" s="128"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="176" t="s">
+      <c r="C7" s="172" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="177"/>
+      <c r="D7" s="173"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -9323,7 +9514,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="28"/>
-      <c r="M8" s="130" t="s">
+      <c r="M8" s="121" t="s">
         <v>10</v>
       </c>
       <c r="N8" s="32" t="s">
@@ -9349,49 +9540,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="118">
+      <c r="A9" s="120">
         <v>90</v>
       </c>
-      <c r="B9" s="118">
+      <c r="B9" s="120">
         <v>3500</v>
       </c>
-      <c r="C9" s="118">
+      <c r="C9" s="120">
         <v>170</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D9" s="120">
         <v>17</v>
       </c>
-      <c r="E9" s="118">
+      <c r="E9" s="120">
         <v>-10</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="120">
         <v>95</v>
       </c>
-      <c r="G9" s="117">
+      <c r="G9" s="119">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C9-A9))*(D9/F9)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H9" s="117">
+      <c r="H9" s="119">
         <f>IFERROR(ROUND(MOD(A9+G9,360),0),"")</f>
         <v>100</v>
       </c>
-      <c r="I9" s="118">
+      <c r="I9" s="120">
         <v>13</v>
       </c>
-      <c r="J9" s="117">
+      <c r="J9" s="119">
         <f>IFERROR(MOD(H9+I9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="K9" s="118">
+      <c r="K9" s="120">
         <v>0</v>
       </c>
       <c r="L9" s="29"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="117">
+      <c r="M9" s="122"/>
+      <c r="N9" s="119">
         <f>IFERROR(MOD(J9+K9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="O9" s="118">
+      <c r="O9" s="120">
         <v>7</v>
       </c>
       <c r="P9" s="42">
@@ -9416,23 +9607,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="118"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="118"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="120"/>
       <c r="L10" s="29"/>
-      <c r="M10" s="114" t="s">
+      <c r="M10" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="117"/>
-      <c r="O10" s="118"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="120"/>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="45"/>
@@ -9440,49 +9631,49 @@
       <c r="T10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="123">
+      <c r="A11" s="118">
         <v>90</v>
       </c>
-      <c r="B11" s="123">
+      <c r="B11" s="118">
         <v>3500</v>
       </c>
-      <c r="C11" s="123">
+      <c r="C11" s="118">
         <v>215</v>
       </c>
-      <c r="D11" s="123">
+      <c r="D11" s="118">
         <v>17</v>
       </c>
-      <c r="E11" s="123">
+      <c r="E11" s="118">
         <v>-10</v>
       </c>
-      <c r="F11" s="123">
+      <c r="F11" s="118">
         <v>95</v>
       </c>
-      <c r="G11" s="121">
+      <c r="G11" s="117">
         <f t="shared" ref="G11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C11-A11))*(D11/F11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="H11" s="121">
+      <c r="H11" s="117">
         <f t="shared" ref="H11" si="1">IFERROR(ROUND(MOD(A11+G11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="I11" s="123">
+      <c r="I11" s="118">
         <v>13</v>
       </c>
-      <c r="J11" s="121">
+      <c r="J11" s="117">
         <f t="shared" ref="J11" si="2">IFERROR(MOD(H11+I11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="K11" s="123">
+      <c r="K11" s="118">
         <v>0</v>
       </c>
       <c r="L11" s="29"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="121">
+      <c r="M11" s="122"/>
+      <c r="N11" s="117">
         <f>IFERROR(MOD(J11+K11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="123">
+      <c r="O11" s="118">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -9507,23 +9698,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="123"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="121"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="121"/>
-      <c r="K12" s="123"/>
+      <c r="A12" s="118"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="118"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="114" t="s">
+      <c r="M12" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="121"/>
-      <c r="O12" s="123"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="118"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -9531,49 +9722,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="118">
+      <c r="A13" s="120">
         <v>131</v>
       </c>
-      <c r="B13" s="118">
+      <c r="B13" s="120">
         <v>3500</v>
       </c>
-      <c r="C13" s="118">
+      <c r="C13" s="120">
         <v>215</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D13" s="120">
         <v>17</v>
       </c>
-      <c r="E13" s="118">
+      <c r="E13" s="120">
         <v>-10</v>
       </c>
-      <c r="F13" s="118">
+      <c r="F13" s="120">
         <v>95</v>
       </c>
-      <c r="G13" s="117">
+      <c r="G13" s="119">
         <f t="shared" ref="G13" si="4">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C13-A13))*(D13/F13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H13" s="117">
+      <c r="H13" s="119">
         <f t="shared" ref="H13" si="5">IFERROR(ROUND(MOD(A13+G13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I13" s="118">
+      <c r="I13" s="120">
         <v>13</v>
       </c>
-      <c r="J13" s="117">
+      <c r="J13" s="119">
         <f t="shared" ref="J13" si="6">IFERROR(MOD(H13+I13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K13" s="118">
+      <c r="K13" s="120">
         <v>2</v>
       </c>
       <c r="L13" s="29"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="117">
+      <c r="M13" s="122"/>
+      <c r="N13" s="119">
         <f>IFERROR(MOD(J13+K13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="118">
+      <c r="O13" s="120">
         <v>11</v>
       </c>
       <c r="P13" s="42">
@@ -9598,23 +9789,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="118"/>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="117"/>
-      <c r="K14" s="118"/>
+      <c r="A14" s="120"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="120"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="114" t="s">
+      <c r="M14" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="117"/>
-      <c r="O14" s="118"/>
+      <c r="N14" s="119"/>
+      <c r="O14" s="120"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
       <c r="R14" s="45"/>
@@ -9622,49 +9813,49 @@
       <c r="T14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="116">
+      <c r="A15" s="131">
         <v>131</v>
       </c>
-      <c r="B15" s="116">
+      <c r="B15" s="131">
         <v>3500</v>
       </c>
-      <c r="C15" s="116">
+      <c r="C15" s="131">
         <v>215</v>
       </c>
-      <c r="D15" s="116">
+      <c r="D15" s="131">
         <v>17</v>
       </c>
-      <c r="E15" s="116">
+      <c r="E15" s="131">
         <v>-10</v>
       </c>
-      <c r="F15" s="116">
+      <c r="F15" s="131">
         <v>95</v>
       </c>
-      <c r="G15" s="121">
+      <c r="G15" s="117">
         <f t="shared" ref="G15" si="8">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C15-A15))*(D15/F15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H15" s="121">
+      <c r="H15" s="117">
         <f t="shared" ref="H15" si="9">IFERROR(ROUND(MOD(A15+G15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I15" s="123">
+      <c r="I15" s="118">
         <v>13</v>
       </c>
-      <c r="J15" s="121">
+      <c r="J15" s="117">
         <f t="shared" ref="J15" si="10">IFERROR(MOD(H15+I15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K15" s="123">
+      <c r="K15" s="118">
         <v>2</v>
       </c>
       <c r="L15" s="29"/>
-      <c r="M15" s="115"/>
-      <c r="N15" s="121">
+      <c r="M15" s="122"/>
+      <c r="N15" s="117">
         <f>IFERROR(MOD(J15+K15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="123">
+      <c r="O15" s="118">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -9689,23 +9880,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="116"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="123"/>
+      <c r="A16" s="131"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="117"/>
+      <c r="K16" s="118"/>
       <c r="L16" s="29"/>
-      <c r="M16" s="114" t="s">
+      <c r="M16" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="121"/>
-      <c r="O16" s="123"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="118"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -9713,49 +9904,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="118">
+      <c r="A17" s="120">
         <v>131</v>
       </c>
-      <c r="B17" s="118">
+      <c r="B17" s="120">
         <v>3500</v>
       </c>
-      <c r="C17" s="118">
+      <c r="C17" s="120">
         <v>215</v>
       </c>
-      <c r="D17" s="118">
+      <c r="D17" s="120">
         <v>17</v>
       </c>
-      <c r="E17" s="118">
+      <c r="E17" s="120">
         <v>-10</v>
       </c>
-      <c r="F17" s="118">
+      <c r="F17" s="120">
         <v>95</v>
       </c>
-      <c r="G17" s="117">
+      <c r="G17" s="119">
         <f t="shared" ref="G17" si="12">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C17-A17))*(D17/F17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H17" s="117">
+      <c r="H17" s="119">
         <f t="shared" ref="H17" si="13">IFERROR(ROUND(MOD(A17+G17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I17" s="118">
+      <c r="I17" s="120">
         <v>13</v>
       </c>
-      <c r="J17" s="117">
+      <c r="J17" s="119">
         <f t="shared" ref="J17" si="14">IFERROR(MOD(H17+I17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K17" s="118">
+      <c r="K17" s="120">
         <v>2</v>
       </c>
       <c r="L17" s="29"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="117">
+      <c r="M17" s="122"/>
+      <c r="N17" s="119">
         <f>IFERROR(MOD(J17+K17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="118">
+      <c r="O17" s="120">
         <v>10</v>
       </c>
       <c r="P17" s="42">
@@ -9780,23 +9971,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="118"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="117"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="118"/>
+      <c r="A18" s="120"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="119"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="120"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="114" t="s">
+      <c r="M18" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="117"/>
-      <c r="O18" s="118"/>
+      <c r="N18" s="119"/>
+      <c r="O18" s="120"/>
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
       <c r="R18" s="45"/>
@@ -9804,49 +9995,49 @@
       <c r="T18" s="44"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="116">
+      <c r="A19" s="131">
         <v>131</v>
       </c>
-      <c r="B19" s="116">
+      <c r="B19" s="131">
         <v>3500</v>
       </c>
-      <c r="C19" s="116">
+      <c r="C19" s="131">
         <v>215</v>
       </c>
-      <c r="D19" s="116">
+      <c r="D19" s="131">
         <v>17</v>
       </c>
-      <c r="E19" s="116">
+      <c r="E19" s="131">
         <v>-10</v>
       </c>
-      <c r="F19" s="116">
+      <c r="F19" s="131">
         <v>95</v>
       </c>
-      <c r="G19" s="121">
+      <c r="G19" s="117">
         <f t="shared" ref="G19" si="16">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C19-A19))*(D19/F19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H19" s="121">
+      <c r="H19" s="117">
         <f t="shared" ref="H19" si="17">IFERROR(ROUND(MOD(A19+G19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I19" s="123">
+      <c r="I19" s="118">
         <v>13</v>
       </c>
-      <c r="J19" s="121">
+      <c r="J19" s="117">
         <f t="shared" ref="J19" si="18">IFERROR(MOD(H19+I19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K19" s="123">
+      <c r="K19" s="118">
         <v>2</v>
       </c>
       <c r="L19" s="29"/>
-      <c r="M19" s="115"/>
-      <c r="N19" s="121">
+      <c r="M19" s="122"/>
+      <c r="N19" s="117">
         <f>IFERROR(MOD(J19+K19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="123">
+      <c r="O19" s="118">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -9871,23 +10062,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="116"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="121"/>
-      <c r="K20" s="123"/>
+      <c r="A20" s="131"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="117"/>
+      <c r="K20" s="118"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="114" t="s">
+      <c r="M20" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="N20" s="121"/>
-      <c r="O20" s="123"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="118"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -9895,33 +10086,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="118"/>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="117" t="str">
+      <c r="A21" s="120"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="119" t="str">
         <f t="shared" ref="G21" si="20">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C21-A21))*(D21/F21)))),0),"")</f>
         <v/>
       </c>
-      <c r="H21" s="117" t="str">
+      <c r="H21" s="119" t="str">
         <f t="shared" ref="H21" si="21">IFERROR(ROUND(MOD(A21+G21,360),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="118"/>
-      <c r="J21" s="117" t="str">
+      <c r="I21" s="120"/>
+      <c r="J21" s="119" t="str">
         <f t="shared" ref="J21" si="22">IFERROR(MOD(H21+I21,360),"")</f>
         <v/>
       </c>
-      <c r="K21" s="118"/>
+      <c r="K21" s="120"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="115"/>
-      <c r="N21" s="117" t="str">
+      <c r="M21" s="122"/>
+      <c r="N21" s="119" t="str">
         <f>IFERROR(MOD(J21+K21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="118"/>
+      <c r="O21" s="120"/>
       <c r="P21" s="42" t="str">
         <f>IFERROR(SQRT(F21^2+D21^2-2*F21*D21*COS(RADIANS(C21-A21-G21))),"")</f>
         <v/>
@@ -9944,21 +10135,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="118"/>
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="118"/>
+      <c r="A22" s="120"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="120"/>
       <c r="L22" s="29"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="118"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="120"/>
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="45"/>
@@ -9966,33 +10157,33 @@
       <c r="T22" s="44"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="116"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="121" t="str">
+      <c r="A23" s="131"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="117" t="str">
         <f t="shared" ref="G23" si="24">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C23-A23))*(D23/F23)))),0),"")</f>
         <v/>
       </c>
-      <c r="H23" s="121" t="str">
+      <c r="H23" s="117" t="str">
         <f t="shared" ref="H23" si="25">IFERROR(ROUND(MOD(A23+G23,360),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="123"/>
-      <c r="J23" s="121" t="str">
+      <c r="I23" s="118"/>
+      <c r="J23" s="117" t="str">
         <f t="shared" ref="J23" si="26">IFERROR(MOD(H23+I23,360),"")</f>
         <v/>
       </c>
-      <c r="K23" s="123"/>
+      <c r="K23" s="118"/>
       <c r="L23" s="29"/>
-      <c r="M23" s="115"/>
-      <c r="N23" s="121" t="str">
+      <c r="M23" s="122"/>
+      <c r="N23" s="117" t="str">
         <f>IFERROR(MOD(J23+K23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="123"/>
+      <c r="O23" s="118"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(F23^2+D23^2-2*F23*D23*COS(RADIANS(C23-A23-G23))),"")</f>
         <v/>
@@ -10015,21 +10206,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="116"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="123"/>
-      <c r="J24" s="121"/>
-      <c r="K24" s="123"/>
+      <c r="A24" s="131"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="118"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="121"/>
-      <c r="O24" s="123"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="118"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -10037,33 +10228,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="118"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="117" t="str">
+      <c r="A25" s="120"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="120"/>
+      <c r="G25" s="119" t="str">
         <f t="shared" ref="G25" si="28">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C25-A25))*(D25/F25)))),0),"")</f>
         <v/>
       </c>
-      <c r="H25" s="117" t="str">
+      <c r="H25" s="119" t="str">
         <f t="shared" ref="H25" si="29">IFERROR(ROUND(MOD(A25+G25,360),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="118"/>
-      <c r="J25" s="117" t="str">
+      <c r="I25" s="120"/>
+      <c r="J25" s="119" t="str">
         <f t="shared" ref="J25" si="30">IFERROR(MOD(H25+I25,360),"")</f>
         <v/>
       </c>
-      <c r="K25" s="118"/>
+      <c r="K25" s="120"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="119"/>
-      <c r="N25" s="117" t="str">
+      <c r="M25" s="155"/>
+      <c r="N25" s="119" t="str">
         <f>IFERROR(MOD(J25+K25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="118"/>
+      <c r="O25" s="120"/>
       <c r="P25" s="42" t="str">
         <f>IFERROR(SQRT(F25^2+D25^2-2*F25*D25*COS(RADIANS(C25-A25-G25))),"")</f>
         <v/>
@@ -10086,23 +10277,23 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A26" s="118"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="117"/>
-      <c r="H26" s="117"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="117"/>
-      <c r="K26" s="118"/>
+      <c r="A26" s="120"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="120"/>
+      <c r="G26" s="119"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="120"/>
       <c r="L26" s="29"/>
       <c r="M26" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N26" s="117"/>
-      <c r="O26" s="118"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="120"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
       <c r="R26" s="45"/>
@@ -10110,19 +10301,19 @@
       <c r="T26" s="44"/>
     </row>
     <row r="27" spans="1:20" ht="25.5" thickBot="1">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="97"/>
-      <c r="K27" s="98"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="138"/>
+      <c r="J27" s="138"/>
+      <c r="K27" s="139"/>
       <c r="L27" s="30"/>
       <c r="M27" s="31" t="s">
         <v>67</v>
@@ -10145,23 +10336,143 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A28" s="99"/>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="100"/>
-      <c r="K28" s="101"/>
+      <c r="A28" s="140"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="142"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="144">
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A27:K28"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
@@ -10186,126 +10497,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="A27:K28"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="N6:T6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -10315,11 +10506,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CFACEB-C7F9-4EC2-B331-5938690C3313}">
-  <dimension ref="B1:J46"/>
+  <dimension ref="B1:V46"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10333,8 +10522,8 @@
     <col min="10" max="10" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="19.5">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:22" ht="20.25" thickBot="1">
       <c r="B2" s="178" t="s">
         <v>96</v>
       </c>
@@ -10346,8 +10535,11 @@
       <c r="H2" s="179"/>
       <c r="I2" s="179"/>
       <c r="J2" s="180"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="L2" s="186" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22">
       <c r="B3" s="66"/>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
@@ -10357,8 +10549,21 @@
       <c r="H3" s="67"/>
       <c r="I3" s="67"/>
       <c r="J3" s="68"/>
-    </row>
-    <row r="4" spans="2:10" ht="18.75">
+      <c r="L3" s="187" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
+      <c r="O3" s="188"/>
+      <c r="P3" s="188"/>
+      <c r="Q3" s="188"/>
+      <c r="R3" s="188"/>
+      <c r="S3" s="188"/>
+      <c r="T3" s="188"/>
+      <c r="U3" s="188"/>
+      <c r="V3" s="189"/>
+    </row>
+    <row r="4" spans="2:22" ht="18.75">
       <c r="B4" s="66"/>
       <c r="C4" s="77" t="s">
         <v>83</v>
@@ -10379,8 +10584,19 @@
       </c>
       <c r="I4" s="69"/>
       <c r="J4" s="68"/>
-    </row>
-    <row r="5" spans="2:10" ht="18.75">
+      <c r="L4" s="190"/>
+      <c r="M4" s="191"/>
+      <c r="N4" s="191"/>
+      <c r="O4" s="191"/>
+      <c r="P4" s="191"/>
+      <c r="Q4" s="191"/>
+      <c r="R4" s="191"/>
+      <c r="S4" s="191"/>
+      <c r="T4" s="191"/>
+      <c r="U4" s="191"/>
+      <c r="V4" s="192"/>
+    </row>
+    <row r="5" spans="2:22" ht="18.75">
       <c r="B5" s="66"/>
       <c r="C5" s="89" t="s">
         <v>95</v>
@@ -10401,8 +10617,19 @@
       </c>
       <c r="I5" s="69"/>
       <c r="J5" s="68"/>
-    </row>
-    <row r="6" spans="2:10" ht="18.75">
+      <c r="L5" s="190"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="191"/>
+      <c r="S5" s="191"/>
+      <c r="T5" s="191"/>
+      <c r="U5" s="191"/>
+      <c r="V5" s="192"/>
+    </row>
+    <row r="6" spans="2:22" ht="18.75">
       <c r="B6" s="66"/>
       <c r="C6" s="79" t="s">
         <v>88</v>
@@ -10416,8 +10643,19 @@
       <c r="H6" s="69"/>
       <c r="I6" s="69"/>
       <c r="J6" s="68"/>
-    </row>
-    <row r="7" spans="2:10" ht="18.75">
+      <c r="L6" s="190"/>
+      <c r="M6" s="191"/>
+      <c r="N6" s="191"/>
+      <c r="O6" s="191"/>
+      <c r="P6" s="191"/>
+      <c r="Q6" s="191"/>
+      <c r="R6" s="191"/>
+      <c r="S6" s="191"/>
+      <c r="T6" s="191"/>
+      <c r="U6" s="191"/>
+      <c r="V6" s="192"/>
+    </row>
+    <row r="7" spans="2:22" ht="18.75">
       <c r="B7" s="66"/>
       <c r="C7" s="81" t="s">
         <v>87</v>
@@ -10438,8 +10676,19 @@
       </c>
       <c r="I7" s="69"/>
       <c r="J7" s="68"/>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="L7" s="190"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
+      <c r="O7" s="191"/>
+      <c r="P7" s="191"/>
+      <c r="Q7" s="191"/>
+      <c r="R7" s="191"/>
+      <c r="S7" s="191"/>
+      <c r="T7" s="191"/>
+      <c r="U7" s="191"/>
+      <c r="V7" s="192"/>
+    </row>
+    <row r="8" spans="2:22">
       <c r="B8" s="66"/>
       <c r="C8" s="67"/>
       <c r="D8" s="67"/>
@@ -10456,8 +10705,19 @@
       </c>
       <c r="I8" s="69"/>
       <c r="J8" s="68"/>
-    </row>
-    <row r="9" spans="2:10">
+      <c r="L8" s="190"/>
+      <c r="M8" s="191"/>
+      <c r="N8" s="191"/>
+      <c r="O8" s="191"/>
+      <c r="P8" s="191"/>
+      <c r="Q8" s="191"/>
+      <c r="R8" s="191"/>
+      <c r="S8" s="191"/>
+      <c r="T8" s="191"/>
+      <c r="U8" s="191"/>
+      <c r="V8" s="192"/>
+    </row>
+    <row r="9" spans="2:22">
       <c r="B9" s="66"/>
       <c r="C9" s="67"/>
       <c r="D9" s="67"/>
@@ -10467,8 +10727,19 @@
       <c r="H9" s="67"/>
       <c r="I9" s="67"/>
       <c r="J9" s="68"/>
-    </row>
-    <row r="10" spans="2:10" ht="18.75">
+      <c r="L9" s="190"/>
+      <c r="M9" s="191"/>
+      <c r="N9" s="191"/>
+      <c r="O9" s="191"/>
+      <c r="P9" s="191"/>
+      <c r="Q9" s="191"/>
+      <c r="R9" s="191"/>
+      <c r="S9" s="191"/>
+      <c r="T9" s="191"/>
+      <c r="U9" s="191"/>
+      <c r="V9" s="192"/>
+    </row>
+    <row r="10" spans="2:22" ht="18.75">
       <c r="B10" s="66"/>
       <c r="C10" s="185" t="s">
         <v>23</v>
@@ -10480,8 +10751,19 @@
       <c r="H10" s="67"/>
       <c r="I10" s="67"/>
       <c r="J10" s="68"/>
-    </row>
-    <row r="11" spans="2:10" ht="18.75">
+      <c r="L10" s="190"/>
+      <c r="M10" s="191"/>
+      <c r="N10" s="191"/>
+      <c r="O10" s="191"/>
+      <c r="P10" s="191"/>
+      <c r="Q10" s="191"/>
+      <c r="R10" s="191"/>
+      <c r="S10" s="191"/>
+      <c r="T10" s="191"/>
+      <c r="U10" s="191"/>
+      <c r="V10" s="192"/>
+    </row>
+    <row r="11" spans="2:22" ht="19.5" thickBot="1">
       <c r="B11" s="66"/>
       <c r="C11" s="184">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(Wd-HEading))*(Ws/TrueAirSpeed)))),0),"")</f>
@@ -10494,8 +10776,19 @@
       <c r="H11" s="67"/>
       <c r="I11" s="67"/>
       <c r="J11" s="68"/>
-    </row>
-    <row r="12" spans="2:10">
+      <c r="L11" s="193"/>
+      <c r="M11" s="194"/>
+      <c r="N11" s="194"/>
+      <c r="O11" s="194"/>
+      <c r="P11" s="194"/>
+      <c r="Q11" s="194"/>
+      <c r="R11" s="194"/>
+      <c r="S11" s="194"/>
+      <c r="T11" s="194"/>
+      <c r="U11" s="194"/>
+      <c r="V11" s="195"/>
+    </row>
+    <row r="12" spans="2:22">
       <c r="B12" s="66"/>
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
@@ -10506,7 +10799,7 @@
       <c r="I12" s="67"/>
       <c r="J12" s="68"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:22">
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
       <c r="D13" s="67"/>
@@ -10517,7 +10810,7 @@
       <c r="I13" s="67"/>
       <c r="J13" s="68"/>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:22">
       <c r="B14" s="66"/>
       <c r="C14" s="67"/>
       <c r="D14" s="67"/>
@@ -10528,7 +10821,7 @@
       <c r="I14" s="67"/>
       <c r="J14" s="68"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:22">
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
       <c r="D15" s="67"/>
@@ -10539,7 +10832,7 @@
       <c r="I15" s="67"/>
       <c r="J15" s="68"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:22">
       <c r="B16" s="66"/>
       <c r="C16" s="67"/>
       <c r="D16" s="67"/>
@@ -10550,7 +10843,7 @@
       <c r="I16" s="67"/>
       <c r="J16" s="68"/>
     </row>
-    <row r="17" spans="2:10" ht="19.5">
+    <row r="17" spans="2:22" ht="19.5">
       <c r="B17" s="181" t="s">
         <v>97</v>
       </c>
@@ -10563,7 +10856,7 @@
       <c r="I17" s="182"/>
       <c r="J17" s="183"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1">
+    <row r="18" spans="2:22" ht="15.75" thickBot="1">
       <c r="B18" s="66"/>
       <c r="C18" s="67"/>
       <c r="D18" s="67"/>
@@ -10574,7 +10867,7 @@
       <c r="I18" s="67"/>
       <c r="J18" s="68"/>
     </row>
-    <row r="19" spans="2:10" ht="19.5" thickBot="1">
+    <row r="19" spans="2:22" ht="19.5" thickBot="1">
       <c r="B19" s="66"/>
       <c r="C19" s="74" t="s">
         <v>86</v>
@@ -10595,8 +10888,11 @@
       </c>
       <c r="I19" s="67"/>
       <c r="J19" s="68"/>
-    </row>
-    <row r="20" spans="2:10" ht="19.5" thickBot="1">
+      <c r="L19" s="186" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" ht="19.5" customHeight="1" thickBot="1">
       <c r="B20" s="66"/>
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
@@ -10613,8 +10909,21 @@
       </c>
       <c r="I20" s="67"/>
       <c r="J20" s="68"/>
-    </row>
-    <row r="21" spans="2:10">
+      <c r="L20" s="187" t="s">
+        <v>100</v>
+      </c>
+      <c r="M20" s="196"/>
+      <c r="N20" s="196"/>
+      <c r="O20" s="196"/>
+      <c r="P20" s="196"/>
+      <c r="Q20" s="196"/>
+      <c r="R20" s="196"/>
+      <c r="S20" s="196"/>
+      <c r="T20" s="196"/>
+      <c r="U20" s="196"/>
+      <c r="V20" s="197"/>
+    </row>
+    <row r="21" spans="2:22">
       <c r="B21" s="66"/>
       <c r="C21" s="67"/>
       <c r="D21" s="67"/>
@@ -10626,8 +10935,19 @@
       <c r="H21" s="67"/>
       <c r="I21" s="67"/>
       <c r="J21" s="68"/>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="L21" s="198"/>
+      <c r="M21" s="199"/>
+      <c r="N21" s="199"/>
+      <c r="O21" s="199"/>
+      <c r="P21" s="199"/>
+      <c r="Q21" s="199"/>
+      <c r="R21" s="199"/>
+      <c r="S21" s="199"/>
+      <c r="T21" s="199"/>
+      <c r="U21" s="199"/>
+      <c r="V21" s="200"/>
+    </row>
+    <row r="22" spans="2:22">
       <c r="B22" s="66"/>
       <c r="C22" s="67"/>
       <c r="D22" s="67"/>
@@ -10637,8 +10957,19 @@
       <c r="H22" s="67"/>
       <c r="I22" s="67"/>
       <c r="J22" s="68"/>
-    </row>
-    <row r="23" spans="2:10">
+      <c r="L22" s="198"/>
+      <c r="M22" s="199"/>
+      <c r="N22" s="199"/>
+      <c r="O22" s="199"/>
+      <c r="P22" s="199"/>
+      <c r="Q22" s="199"/>
+      <c r="R22" s="199"/>
+      <c r="S22" s="199"/>
+      <c r="T22" s="199"/>
+      <c r="U22" s="199"/>
+      <c r="V22" s="200"/>
+    </row>
+    <row r="23" spans="2:22">
       <c r="B23" s="66"/>
       <c r="C23" s="69" t="s">
         <v>90</v>
@@ -10656,8 +10987,19 @@
       <c r="H23" s="67"/>
       <c r="I23" s="67"/>
       <c r="J23" s="68"/>
-    </row>
-    <row r="24" spans="2:10">
+      <c r="L23" s="198"/>
+      <c r="M23" s="199"/>
+      <c r="N23" s="199"/>
+      <c r="O23" s="199"/>
+      <c r="P23" s="199"/>
+      <c r="Q23" s="199"/>
+      <c r="R23" s="199"/>
+      <c r="S23" s="199"/>
+      <c r="T23" s="199"/>
+      <c r="U23" s="199"/>
+      <c r="V23" s="200"/>
+    </row>
+    <row r="24" spans="2:22">
       <c r="B24" s="66"/>
       <c r="C24" s="69" t="s">
         <v>91</v>
@@ -10675,8 +11017,19 @@
       <c r="H24" s="67"/>
       <c r="I24" s="67"/>
       <c r="J24" s="68"/>
-    </row>
-    <row r="25" spans="2:10">
+      <c r="L24" s="198"/>
+      <c r="M24" s="199"/>
+      <c r="N24" s="199"/>
+      <c r="O24" s="199"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="199"/>
+      <c r="R24" s="199"/>
+      <c r="S24" s="199"/>
+      <c r="T24" s="199"/>
+      <c r="U24" s="199"/>
+      <c r="V24" s="200"/>
+    </row>
+    <row r="25" spans="2:22">
       <c r="B25" s="66"/>
       <c r="C25" s="67"/>
       <c r="D25" s="67"/>
@@ -10686,8 +11039,19 @@
       <c r="H25" s="67"/>
       <c r="I25" s="67"/>
       <c r="J25" s="68"/>
-    </row>
-    <row r="26" spans="2:10">
+      <c r="L25" s="198"/>
+      <c r="M25" s="199"/>
+      <c r="N25" s="199"/>
+      <c r="O25" s="199"/>
+      <c r="P25" s="199"/>
+      <c r="Q25" s="199"/>
+      <c r="R25" s="199"/>
+      <c r="S25" s="199"/>
+      <c r="T25" s="199"/>
+      <c r="U25" s="199"/>
+      <c r="V25" s="200"/>
+    </row>
+    <row r="26" spans="2:22">
       <c r="B26" s="66"/>
       <c r="C26" s="67"/>
       <c r="D26" s="67"/>
@@ -10697,8 +11061,19 @@
       <c r="H26" s="67"/>
       <c r="I26" s="67"/>
       <c r="J26" s="68"/>
-    </row>
-    <row r="27" spans="2:10">
+      <c r="L26" s="198"/>
+      <c r="M26" s="199"/>
+      <c r="N26" s="199"/>
+      <c r="O26" s="199"/>
+      <c r="P26" s="199"/>
+      <c r="Q26" s="199"/>
+      <c r="R26" s="199"/>
+      <c r="S26" s="199"/>
+      <c r="T26" s="199"/>
+      <c r="U26" s="199"/>
+      <c r="V26" s="200"/>
+    </row>
+    <row r="27" spans="2:22">
       <c r="B27" s="66"/>
       <c r="C27" s="67"/>
       <c r="D27" s="67"/>
@@ -10708,8 +11083,19 @@
       <c r="H27" s="67"/>
       <c r="I27" s="67"/>
       <c r="J27" s="68"/>
-    </row>
-    <row r="28" spans="2:10">
+      <c r="L27" s="198"/>
+      <c r="M27" s="199"/>
+      <c r="N27" s="199"/>
+      <c r="O27" s="199"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="199"/>
+      <c r="R27" s="199"/>
+      <c r="S27" s="199"/>
+      <c r="T27" s="199"/>
+      <c r="U27" s="199"/>
+      <c r="V27" s="200"/>
+    </row>
+    <row r="28" spans="2:22">
       <c r="B28" s="66"/>
       <c r="C28" s="67"/>
       <c r="D28" s="67"/>
@@ -10719,8 +11105,19 @@
       <c r="H28" s="67"/>
       <c r="I28" s="67"/>
       <c r="J28" s="68"/>
-    </row>
-    <row r="29" spans="2:10">
+      <c r="L28" s="198"/>
+      <c r="M28" s="199"/>
+      <c r="N28" s="199"/>
+      <c r="O28" s="199"/>
+      <c r="P28" s="199"/>
+      <c r="Q28" s="199"/>
+      <c r="R28" s="199"/>
+      <c r="S28" s="199"/>
+      <c r="T28" s="199"/>
+      <c r="U28" s="199"/>
+      <c r="V28" s="200"/>
+    </row>
+    <row r="29" spans="2:22">
       <c r="B29" s="66"/>
       <c r="C29" s="67"/>
       <c r="D29" s="67"/>
@@ -10730,8 +11127,19 @@
       <c r="H29" s="67"/>
       <c r="I29" s="67"/>
       <c r="J29" s="68"/>
-    </row>
-    <row r="30" spans="2:10">
+      <c r="L29" s="198"/>
+      <c r="M29" s="199"/>
+      <c r="N29" s="199"/>
+      <c r="O29" s="199"/>
+      <c r="P29" s="199"/>
+      <c r="Q29" s="199"/>
+      <c r="R29" s="199"/>
+      <c r="S29" s="199"/>
+      <c r="T29" s="199"/>
+      <c r="U29" s="199"/>
+      <c r="V29" s="200"/>
+    </row>
+    <row r="30" spans="2:22">
       <c r="B30" s="66"/>
       <c r="C30" s="67"/>
       <c r="D30" s="67"/>
@@ -10741,8 +11149,19 @@
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="J30" s="68"/>
-    </row>
-    <row r="31" spans="2:10">
+      <c r="L30" s="198"/>
+      <c r="M30" s="199"/>
+      <c r="N30" s="199"/>
+      <c r="O30" s="199"/>
+      <c r="P30" s="199"/>
+      <c r="Q30" s="199"/>
+      <c r="R30" s="199"/>
+      <c r="S30" s="199"/>
+      <c r="T30" s="199"/>
+      <c r="U30" s="199"/>
+      <c r="V30" s="200"/>
+    </row>
+    <row r="31" spans="2:22" ht="15.75" thickBot="1">
       <c r="B31" s="66"/>
       <c r="C31" s="67"/>
       <c r="D31" s="67"/>
@@ -10752,8 +11171,19 @@
       <c r="H31" s="67"/>
       <c r="I31" s="67"/>
       <c r="J31" s="68"/>
-    </row>
-    <row r="32" spans="2:10">
+      <c r="L31" s="201"/>
+      <c r="M31" s="202"/>
+      <c r="N31" s="202"/>
+      <c r="O31" s="202"/>
+      <c r="P31" s="202"/>
+      <c r="Q31" s="202"/>
+      <c r="R31" s="202"/>
+      <c r="S31" s="202"/>
+      <c r="T31" s="202"/>
+      <c r="U31" s="202"/>
+      <c r="V31" s="203"/>
+    </row>
+    <row r="32" spans="2:22">
       <c r="B32" s="66"/>
       <c r="C32" s="67"/>
       <c r="D32" s="67"/>
@@ -10920,11 +11350,13 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="L20:V31"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="L3:V11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cross wind component formula explanationo
</commit_message>
<xml_diff>
--- a/NAV Log Calculator - Flight Planner - E6B-like.xlsx
+++ b/NAV Log Calculator - Flight Planner - E6B-like.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/194e8d034589e5e8/Aviation/NAV/Aviation-Navigation-Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="843" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50546B89-F616-4239-B235-D113ADF453BC}"/>
+  <xr:revisionPtr revIDLastSave="848" documentId="13_ncr:1_{462FEA56-7C17-431A-9BAA-3E0293AE842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6B357E3-AF93-40FB-95C3-A4EEEC9B29DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="3" xr2:uid="{81AC26DA-A476-4998-AAF9-3938C858D589}"/>
   </bookViews>
@@ -723,9 +723,12 @@
     </r>
   </si>
   <si>
+    <t>Note about the formula used:</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">The wind makes an angle with the runway. If you treat that wind vector as the hypothenus of a regtangle triangle (this hypothenus length being the wind speed) which adjacent side is the runway, your cross-wind component will be the opposite side of that rectangle triangle - the opposite side being the side which has a 90 degrees angle with the adjacent/runway side. In other words, it's the part of the wind that blows perpendicularily to  the runway and then to the plane when it's aligned to take off. The length of the perpendicular wind component will be the cross wind speed.
-The formula to get the length (aka the force) of that opposite side of that rectangle triangle is :
+      <t xml:space="preserve">The wind vector makes an angle with the runway. If you treat that wind vector as the hypothenus of a right-angled triangle, this hypothenus length being the wind speed, which adjacent side is the runway, your cross-wind component will be the opposite side of that right-angled triangle - the opposite side being the side which has a 90 degrees angle with the adjacent/runway side. In other words, it's the part of the wind that blows perpendicularily to  the runway and then to the plane when it's aligned to take off. The length of the perpendicular wind component will be the cross wind speed.
+The formula to get the length (aka the force) of that opposite side of that right-angled triangle is :
 </t>
     </r>
     <r>
@@ -739,9 +742,6 @@
       </rPr>
       <t>SIN(angle between runway and wind) x Wind speed</t>
     </r>
-  </si>
-  <si>
-    <t>Note about the formula used:</t>
   </si>
 </sst>
 </file>
@@ -1982,6 +1982,154 @@
     <xf numFmtId="0" fontId="45" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2005,13 +2153,7 @@
     <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2047,145 +2189,20 @@
     <xf numFmtId="0" fontId="31" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2216,10 +2233,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2249,17 +2262,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2285,10 +2313,6 @@
     <xf numFmtId="0" fontId="20" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2312,30 +2336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8030,144 +8030,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="113">
+      <c r="B1" s="127">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="128"/>
+      <c r="E1" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="95">
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="141">
         <v>38</v>
       </c>
-      <c r="I1" s="104"/>
+      <c r="I1" s="148"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="107" t="s">
+      <c r="N1" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="108"/>
-      <c r="P1" s="95">
+      <c r="O1" s="152"/>
+      <c r="P1" s="141">
         <v>3500</v>
       </c>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="93" t="s">
+      <c r="Q1" s="141"/>
+      <c r="R1" s="139" t="s">
         <v>70</v>
       </c>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="116"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="105"/>
+      <c r="A2" s="126"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="130"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="149"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="94"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="150"/>
+      <c r="Q2" s="150"/>
+      <c r="R2" s="140"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="95">
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="141">
         <v>6.5</v>
       </c>
-      <c r="I3" s="104"/>
+      <c r="I3" s="148"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="107" t="s">
+      <c r="N3" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="95">
+      <c r="O3" s="152"/>
+      <c r="P3" s="141">
         <v>215</v>
       </c>
-      <c r="Q3" s="97" t="s">
+      <c r="Q3" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="95">
+      <c r="R3" s="141">
         <v>17</v>
       </c>
-      <c r="S3" s="93" t="s">
+      <c r="S3" s="139" t="s">
         <v>71</v>
       </c>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
-      <c r="E4" s="102"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="105"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="98"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="99"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="149"/>
+      <c r="N4" s="155"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="144"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="145"/>
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="136"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="128"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
+      <c r="T6" s="136"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="132" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="129" t="s">
+      <c r="C7" s="133"/>
+      <c r="D7" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="130"/>
+      <c r="E7" s="138"/>
       <c r="F7" s="59" t="s">
         <v>2</v>
       </c>
@@ -8197,7 +8197,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19.7" customHeight="1">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="131" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -8257,49 +8257,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="122"/>
-      <c r="B9" s="120">
+      <c r="A9" s="116"/>
+      <c r="B9" s="119">
         <v>90</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="119">
         <v>3500</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="119">
         <v>215</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="119">
         <v>17</v>
       </c>
-      <c r="F9" s="120">
+      <c r="F9" s="119">
         <v>-10</v>
       </c>
-      <c r="G9" s="120">
+      <c r="G9" s="119">
         <v>95</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="118">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D9-B9))*(E9/G9)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I9" s="119">
+      <c r="I9" s="118">
         <f>IFERROR(ROUND(MOD(B9+H9,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J9" s="120">
+      <c r="J9" s="119">
         <v>13</v>
       </c>
-      <c r="K9" s="119">
+      <c r="K9" s="118">
         <f>IFERROR(MOD(I9+J9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L9" s="120">
+      <c r="L9" s="119">
         <v>0</v>
       </c>
       <c r="M9" s="7"/>
-      <c r="N9" s="119">
+      <c r="N9" s="118">
         <f>IFERROR(MOD(K9+L9,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O9" s="120">
+      <c r="O9" s="119">
         <v>7</v>
       </c>
       <c r="P9" s="43">
@@ -8324,23 +8324,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="123" t="s">
+      <c r="A10" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="120"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="118"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="119"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="120"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="119"/>
       <c r="P10" s="53"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="54"/>
@@ -8348,49 +8348,49 @@
       <c r="T10" s="53"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="122"/>
-      <c r="B11" s="118">
+      <c r="A11" s="116"/>
+      <c r="B11" s="124">
         <v>90</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="124">
         <v>3500</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="124">
         <v>215</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="124">
         <v>17</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="124">
         <v>-10</v>
       </c>
-      <c r="G11" s="118">
+      <c r="G11" s="124">
         <v>95</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="122">
         <f t="shared" ref="H11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D11-B11))*(E11/G11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="I11" s="117">
+      <c r="I11" s="122">
         <f>IFERROR(ROUND(MOD(B11+H11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="J11" s="118">
+      <c r="J11" s="124">
         <v>13</v>
       </c>
-      <c r="K11" s="117">
+      <c r="K11" s="122">
         <f t="shared" ref="K11" si="1">IFERROR(MOD(I11+J11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="L11" s="118">
+      <c r="L11" s="124">
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="117">
+      <c r="N11" s="122">
         <f>IFERROR(MOD(K11+L11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="118">
+      <c r="O11" s="124">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -8415,23 +8415,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="118"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="124"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="118"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="124"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -8439,49 +8439,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="122"/>
-      <c r="B13" s="120">
+      <c r="A13" s="116"/>
+      <c r="B13" s="119">
         <v>131</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C13" s="119">
         <v>3500</v>
       </c>
-      <c r="D13" s="120">
+      <c r="D13" s="119">
         <v>215</v>
       </c>
-      <c r="E13" s="120">
+      <c r="E13" s="119">
         <v>17</v>
       </c>
-      <c r="F13" s="120">
+      <c r="F13" s="119">
         <v>-10</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="119">
         <v>95</v>
       </c>
-      <c r="H13" s="119">
+      <c r="H13" s="118">
         <f t="shared" ref="H13" si="3">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D13-B13))*(E13/G13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I13" s="119">
+      <c r="I13" s="118">
         <f t="shared" ref="I13" si="4">IFERROR(ROUND(MOD(B13+H13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J13" s="120">
+      <c r="J13" s="119">
         <v>13</v>
       </c>
-      <c r="K13" s="119">
+      <c r="K13" s="118">
         <f t="shared" ref="K13" si="5">IFERROR(MOD(I13+J13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L13" s="120">
+      <c r="L13" s="119">
         <v>2</v>
       </c>
       <c r="M13" s="7"/>
-      <c r="N13" s="119">
+      <c r="N13" s="118">
         <f>IFERROR(MOD(K13+L13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="120">
+      <c r="O13" s="119">
         <v>11</v>
       </c>
       <c r="P13" s="43">
@@ -8506,23 +8506,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="123" t="s">
+      <c r="A14" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="120"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="119"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="120"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="119"/>
       <c r="P14" s="53"/>
       <c r="Q14" s="53"/>
       <c r="R14" s="54"/>
@@ -8530,49 +8530,49 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="122"/>
-      <c r="B15" s="131">
+      <c r="A15" s="116"/>
+      <c r="B15" s="117">
         <v>131</v>
       </c>
-      <c r="C15" s="131">
+      <c r="C15" s="117">
         <v>3500</v>
       </c>
-      <c r="D15" s="131">
+      <c r="D15" s="117">
         <v>215</v>
       </c>
-      <c r="E15" s="131">
+      <c r="E15" s="117">
         <v>17</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="117">
         <v>-10</v>
       </c>
-      <c r="G15" s="131">
+      <c r="G15" s="117">
         <v>95</v>
       </c>
-      <c r="H15" s="117">
+      <c r="H15" s="122">
         <f t="shared" ref="H15" si="7">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D15-B15))*(E15/G15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I15" s="117">
+      <c r="I15" s="122">
         <f t="shared" ref="I15" si="8">IFERROR(ROUND(MOD(B15+H15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J15" s="118">
+      <c r="J15" s="124">
         <v>13</v>
       </c>
-      <c r="K15" s="117">
+      <c r="K15" s="122">
         <f t="shared" ref="K15" si="9">IFERROR(MOD(I15+J15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L15" s="118">
+      <c r="L15" s="124">
         <v>2</v>
       </c>
       <c r="M15" s="7"/>
-      <c r="N15" s="117">
+      <c r="N15" s="122">
         <f>IFERROR(MOD(K15+L15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="118">
+      <c r="O15" s="124">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -8597,23 +8597,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="123" t="s">
+      <c r="A16" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="117"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="118"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="122"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="122"/>
+      <c r="L16" s="124"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="118"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="124"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -8621,49 +8621,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="122"/>
-      <c r="B17" s="120">
+      <c r="A17" s="116"/>
+      <c r="B17" s="119">
         <v>131</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="119">
         <v>3500</v>
       </c>
-      <c r="D17" s="120">
+      <c r="D17" s="119">
         <v>215</v>
       </c>
-      <c r="E17" s="120">
+      <c r="E17" s="119">
         <v>17</v>
       </c>
-      <c r="F17" s="120">
+      <c r="F17" s="119">
         <v>-10</v>
       </c>
-      <c r="G17" s="120">
+      <c r="G17" s="119">
         <v>95</v>
       </c>
-      <c r="H17" s="119">
+      <c r="H17" s="118">
         <f t="shared" ref="H17" si="11">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D17-B17))*(E17/G17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I17" s="119">
+      <c r="I17" s="118">
         <f t="shared" ref="I17" si="12">IFERROR(ROUND(MOD(B17+H17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J17" s="120">
+      <c r="J17" s="119">
         <v>13</v>
       </c>
-      <c r="K17" s="119">
+      <c r="K17" s="118">
         <f t="shared" ref="K17" si="13">IFERROR(MOD(I17+J17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L17" s="120">
+      <c r="L17" s="119">
         <v>2</v>
       </c>
       <c r="M17" s="7"/>
-      <c r="N17" s="119">
+      <c r="N17" s="118">
         <f>IFERROR(MOD(K17+L17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="120">
+      <c r="O17" s="119">
         <v>10</v>
       </c>
       <c r="P17" s="43">
@@ -8688,23 +8688,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="123" t="s">
+      <c r="A18" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="120"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="119"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="119"/>
-      <c r="O18" s="120"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="119"/>
       <c r="P18" s="53"/>
       <c r="Q18" s="53"/>
       <c r="R18" s="54"/>
@@ -8712,49 +8712,49 @@
       <c r="T18" s="53"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="122"/>
-      <c r="B19" s="131">
+      <c r="A19" s="116"/>
+      <c r="B19" s="117">
         <v>131</v>
       </c>
-      <c r="C19" s="131">
+      <c r="C19" s="117">
         <v>3500</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="117">
         <v>215</v>
       </c>
-      <c r="E19" s="131">
+      <c r="E19" s="117">
         <v>17</v>
       </c>
-      <c r="F19" s="131">
+      <c r="F19" s="117">
         <v>-10</v>
       </c>
-      <c r="G19" s="131">
+      <c r="G19" s="117">
         <v>95</v>
       </c>
-      <c r="H19" s="117">
+      <c r="H19" s="122">
         <f t="shared" ref="H19" si="15">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D19-B19))*(E19/G19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="I19" s="117">
+      <c r="I19" s="122">
         <f t="shared" ref="I19" si="16">IFERROR(ROUND(MOD(B19+H19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="J19" s="118">
+      <c r="J19" s="124">
         <v>13</v>
       </c>
-      <c r="K19" s="117">
+      <c r="K19" s="122">
         <f t="shared" ref="K19" si="17">IFERROR(MOD(I19+J19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="L19" s="118">
+      <c r="L19" s="124">
         <v>2</v>
       </c>
       <c r="M19" s="7"/>
-      <c r="N19" s="117">
+      <c r="N19" s="122">
         <f>IFERROR(MOD(K19+L19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="118">
+      <c r="O19" s="124">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -8779,23 +8779,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="123" t="s">
+      <c r="A20" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="118"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="122"/>
+      <c r="I20" s="122"/>
+      <c r="J20" s="124"/>
+      <c r="K20" s="122"/>
+      <c r="L20" s="124"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="118"/>
+      <c r="N20" s="122"/>
+      <c r="O20" s="124"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -8803,33 +8803,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="122"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="119" t="str">
+      <c r="A21" s="116"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="119"/>
+      <c r="H21" s="118" t="str">
         <f t="shared" ref="H21" si="19">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D21-B21))*(E21/G21)))),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="119" t="str">
+      <c r="I21" s="118" t="str">
         <f t="shared" ref="I21" si="20">IFERROR(ROUND(MOD(B21+H21,360),0),"")</f>
         <v/>
       </c>
-      <c r="J21" s="120"/>
-      <c r="K21" s="119" t="str">
+      <c r="J21" s="119"/>
+      <c r="K21" s="118" t="str">
         <f t="shared" ref="K21" si="21">IFERROR(MOD(I21+J21,360),"")</f>
         <v/>
       </c>
-      <c r="L21" s="120"/>
+      <c r="L21" s="119"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="119" t="str">
+      <c r="N21" s="118" t="str">
         <f>IFERROR(MOD(K21+L21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="120"/>
+      <c r="O21" s="119"/>
       <c r="P21" s="43" t="str">
         <f>IFERROR(SQRT(G21^2+E21^2-2*G21*E21*COS(RADIANS(D21-B21-H21))),"")</f>
         <v/>
@@ -8852,21 +8852,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="123"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="119"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="119"/>
-      <c r="L22" s="120"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="119"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="119"/>
-      <c r="O22" s="120"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="119"/>
       <c r="P22" s="53"/>
       <c r="Q22" s="53"/>
       <c r="R22" s="54"/>
@@ -8874,33 +8874,33 @@
       <c r="T22" s="53"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="122"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
-      <c r="H23" s="117" t="str">
+      <c r="A23" s="116"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="122" t="str">
         <f t="shared" ref="H23" si="23">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D23-B23))*(E23/G23)))),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="117" t="str">
+      <c r="I23" s="122" t="str">
         <f t="shared" ref="I23" si="24">IFERROR(ROUND(MOD(B23+H23,360),0),"")</f>
         <v/>
       </c>
-      <c r="J23" s="118"/>
-      <c r="K23" s="119" t="str">
+      <c r="J23" s="124"/>
+      <c r="K23" s="118" t="str">
         <f t="shared" ref="K23" si="25">IFERROR(MOD(I23+J23,360),"")</f>
         <v/>
       </c>
-      <c r="L23" s="118"/>
+      <c r="L23" s="124"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="119" t="str">
+      <c r="N23" s="118" t="str">
         <f>IFERROR(MOD(K23+L23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="118"/>
+      <c r="O23" s="124"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(G23^2+E23^2-2*G23*E23*COS(RADIANS(D23-B23-H23))),"")</f>
         <v/>
@@ -8923,21 +8923,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="123"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="131"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="119"/>
-      <c r="L24" s="118"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="124"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="124"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="119"/>
-      <c r="O24" s="118"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="124"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -8945,33 +8945,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="155"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="119" t="str">
+      <c r="A25" s="120"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="119"/>
+      <c r="H25" s="118" t="str">
         <f t="shared" ref="H25" si="27">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(D25-B25))*(E25/G25)))),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="119" t="str">
+      <c r="I25" s="118" t="str">
         <f t="shared" ref="I25" si="28">IFERROR(ROUND(MOD(B25+H25,360),0),"")</f>
         <v/>
       </c>
-      <c r="J25" s="120"/>
-      <c r="K25" s="119" t="str">
+      <c r="J25" s="119"/>
+      <c r="K25" s="118" t="str">
         <f t="shared" ref="K25" si="29">IFERROR(MOD(I25+J25,360),"")</f>
         <v/>
       </c>
-      <c r="L25" s="120"/>
+      <c r="L25" s="119"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="119" t="str">
+      <c r="N25" s="118" t="str">
         <f>IFERROR(MOD(K25+L25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="120"/>
+      <c r="O25" s="119"/>
       <c r="P25" s="43" t="str">
         <f>IFERROR(SQRT(G25^2+E25^2-2*G25*E25*COS(RADIANS(D25-B25-H25))),"")</f>
         <v/>
@@ -8997,20 +8997,20 @@
       <c r="A26" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="133"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="132"/>
-      <c r="K26" s="133"/>
-      <c r="L26" s="132"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="123"/>
+      <c r="I26" s="123"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="123"/>
+      <c r="L26" s="121"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="132"/>
+      <c r="N26" s="118"/>
+      <c r="O26" s="121"/>
       <c r="P26" s="53"/>
       <c r="Q26" s="55"/>
       <c r="R26" s="56"/>
@@ -9018,130 +9018,256 @@
       <c r="T26" s="53"/>
     </row>
     <row r="27" spans="1:20" ht="15" customHeight="1">
-      <c r="A27" s="149" t="s">
+      <c r="A27" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="150"/>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="150"/>
-      <c r="K27" s="150"/>
-      <c r="L27" s="151"/>
-      <c r="O27" s="143">
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="111"/>
+      <c r="O27" s="103">
         <f>SUM(O9:O26)</f>
         <v>55</v>
       </c>
-      <c r="Q27" s="145">
+      <c r="Q27" s="105">
         <f>SUM(Q9:Q26)</f>
         <v>35</v>
       </c>
-      <c r="R27" s="147">
+      <c r="R27" s="107">
         <f>MAX(R9:R26)</f>
         <v>0.60763888888888895</v>
       </c>
-      <c r="S27" s="145">
+      <c r="S27" s="105">
         <f>SUM(S9:S26)</f>
         <v>3.8</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="152"/>
-      <c r="B28" s="153"/>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="153"/>
-      <c r="J28" s="153"/>
-      <c r="K28" s="153"/>
-      <c r="L28" s="154"/>
-      <c r="O28" s="144"/>
-      <c r="Q28" s="146"/>
-      <c r="R28" s="148"/>
-      <c r="S28" s="146"/>
+      <c r="A28" s="112"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="113"/>
+      <c r="L28" s="114"/>
+      <c r="O28" s="104"/>
+      <c r="Q28" s="106"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="106"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="135"/>
-      <c r="C29" s="135"/>
-      <c r="D29" s="135"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
-      <c r="G29" s="135"/>
-      <c r="H29" s="135"/>
-      <c r="I29" s="135"/>
-      <c r="J29" s="135"/>
-      <c r="K29" s="135"/>
-      <c r="L29" s="136"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="96"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="137"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="138"/>
-      <c r="J30" s="138"/>
-      <c r="K30" s="138"/>
-      <c r="L30" s="139"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="99"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="137"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="138"/>
-      <c r="J31" s="138"/>
-      <c r="K31" s="138"/>
-      <c r="L31" s="139"/>
+      <c r="A31" s="97"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
+      <c r="K31" s="98"/>
+      <c r="L31" s="99"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="137"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="138"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="138"/>
-      <c r="J32" s="138"/>
-      <c r="K32" s="138"/>
-      <c r="L32" s="139"/>
+      <c r="A32" s="97"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="99"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="140"/>
-      <c r="B33" s="141"/>
-      <c r="C33" s="141"/>
-      <c r="D33" s="141"/>
-      <c r="E33" s="141"/>
-      <c r="F33" s="141"/>
-      <c r="G33" s="141"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
-      <c r="J33" s="141"/>
-      <c r="K33" s="141"/>
-      <c r="L33" s="142"/>
+      <c r="A33" s="100"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="102"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="150">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E1:G2"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="A29:L33"/>
     <mergeCell ref="O27:O28"/>
     <mergeCell ref="Q27:Q28"/>
@@ -9166,132 +9292,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E1:G2"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="N3:O4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
@@ -9324,134 +9324,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="160">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="166">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E1" s="161"/>
+      <c r="E1" s="167"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="165" t="s">
+      <c r="G1" s="170" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="164">
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="161">
         <v>38</v>
       </c>
-      <c r="K1" s="164"/>
+      <c r="K1" s="161"/>
       <c r="L1" s="24"/>
-      <c r="M1" s="166" t="s">
+      <c r="M1" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="168">
+      <c r="N1" s="173">
         <v>3500</v>
       </c>
-      <c r="O1" s="168"/>
-      <c r="P1" s="174" t="s">
+      <c r="O1" s="173"/>
+      <c r="P1" s="157" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="158"/>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="A2" s="164"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="161"/>
+      <c r="K2" s="161"/>
       <c r="L2" s="24"/>
-      <c r="M2" s="167"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="175"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="161"/>
+      <c r="O2" s="161"/>
+      <c r="P2" s="158"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
-      <c r="G3" s="165" t="s">
+      <c r="G3" s="170" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
-      <c r="J3" s="164">
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="161">
         <v>6.5</v>
       </c>
-      <c r="K3" s="164"/>
+      <c r="K3" s="161"/>
       <c r="L3" s="25"/>
-      <c r="M3" s="169" t="s">
+      <c r="M3" s="174" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="164">
+      <c r="N3" s="161">
         <v>215</v>
       </c>
-      <c r="O3" s="164"/>
-      <c r="P3" s="176" t="s">
+      <c r="O3" s="161"/>
+      <c r="P3" s="159" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="164">
+      <c r="Q3" s="161">
         <v>17</v>
       </c>
-      <c r="R3" s="164"/>
-      <c r="S3" s="174" t="s">
+      <c r="R3" s="161"/>
+      <c r="S3" s="157" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="164"/>
-      <c r="K4" s="164"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="170"/>
+      <c r="I4" s="170"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
       <c r="L4" s="25"/>
-      <c r="M4" s="170"/>
-      <c r="N4" s="171"/>
-      <c r="O4" s="171"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="164"/>
-      <c r="R4" s="164"/>
-      <c r="S4" s="175"/>
+      <c r="M4" s="175"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="176"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="158"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1">
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="128"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="136"/>
       <c r="L6" s="26"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="126" t="s">
+      <c r="N6" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="128"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
+      <c r="T6" s="136"/>
     </row>
     <row r="7" spans="1:20" ht="19.7" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="172" t="s">
+      <c r="C7" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="173"/>
+      <c r="D7" s="178"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -9514,7 +9514,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="28"/>
-      <c r="M8" s="121" t="s">
+      <c r="M8" s="131" t="s">
         <v>10</v>
       </c>
       <c r="N8" s="32" t="s">
@@ -9540,49 +9540,49 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A9" s="120">
+      <c r="A9" s="119">
         <v>90</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="119">
         <v>3500</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="119">
         <v>170</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="119">
         <v>17</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="119">
         <v>-10</v>
       </c>
-      <c r="F9" s="120">
+      <c r="F9" s="119">
         <v>95</v>
       </c>
-      <c r="G9" s="119">
+      <c r="G9" s="118">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C9-A9))*(D9/F9)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="118">
         <f>IFERROR(ROUND(MOD(A9+G9,360),0),"")</f>
         <v>100</v>
       </c>
-      <c r="I9" s="120">
+      <c r="I9" s="119">
         <v>13</v>
       </c>
-      <c r="J9" s="119">
+      <c r="J9" s="118">
         <f>IFERROR(MOD(H9+I9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="K9" s="120">
+      <c r="K9" s="119">
         <v>0</v>
       </c>
       <c r="L9" s="29"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="119">
+      <c r="M9" s="116"/>
+      <c r="N9" s="118">
         <f>IFERROR(MOD(J9+K9,360),"")</f>
         <v>113</v>
       </c>
-      <c r="O9" s="120">
+      <c r="O9" s="119">
         <v>7</v>
       </c>
       <c r="P9" s="42">
@@ -9607,23 +9607,23 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A10" s="120"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="120"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="119"/>
       <c r="L10" s="29"/>
-      <c r="M10" s="123" t="s">
+      <c r="M10" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="119"/>
-      <c r="O10" s="120"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="119"/>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="45"/>
@@ -9631,49 +9631,49 @@
       <c r="T10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A11" s="118">
+      <c r="A11" s="124">
         <v>90</v>
       </c>
-      <c r="B11" s="118">
+      <c r="B11" s="124">
         <v>3500</v>
       </c>
-      <c r="C11" s="118">
+      <c r="C11" s="124">
         <v>215</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="124">
         <v>17</v>
       </c>
-      <c r="E11" s="118">
+      <c r="E11" s="124">
         <v>-10</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="124">
         <v>95</v>
       </c>
-      <c r="G11" s="117">
+      <c r="G11" s="122">
         <f t="shared" ref="G11" si="0">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C11-A11))*(D11/F11)))),0),"")</f>
         <v>8</v>
       </c>
-      <c r="H11" s="117">
+      <c r="H11" s="122">
         <f t="shared" ref="H11" si="1">IFERROR(ROUND(MOD(A11+G11,360),0),"")</f>
         <v>98</v>
       </c>
-      <c r="I11" s="118">
+      <c r="I11" s="124">
         <v>13</v>
       </c>
-      <c r="J11" s="117">
+      <c r="J11" s="122">
         <f t="shared" ref="J11" si="2">IFERROR(MOD(H11+I11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="K11" s="118">
+      <c r="K11" s="124">
         <v>0</v>
       </c>
       <c r="L11" s="29"/>
-      <c r="M11" s="122"/>
-      <c r="N11" s="117">
+      <c r="M11" s="116"/>
+      <c r="N11" s="122">
         <f>IFERROR(MOD(J11+K11,360),"")</f>
         <v>111</v>
       </c>
-      <c r="O11" s="118">
+      <c r="O11" s="124">
         <v>8</v>
       </c>
       <c r="P11" s="46">
@@ -9698,23 +9698,23 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A12" s="118"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="118"/>
+      <c r="A12" s="124"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="124"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="123" t="s">
+      <c r="M12" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="117"/>
-      <c r="O12" s="118"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="124"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="44"/>
       <c r="R12" s="45"/>
@@ -9722,49 +9722,49 @@
       <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="120">
+      <c r="A13" s="119">
         <v>131</v>
       </c>
-      <c r="B13" s="120">
+      <c r="B13" s="119">
         <v>3500</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C13" s="119">
         <v>215</v>
       </c>
-      <c r="D13" s="120">
+      <c r="D13" s="119">
         <v>17</v>
       </c>
-      <c r="E13" s="120">
+      <c r="E13" s="119">
         <v>-10</v>
       </c>
-      <c r="F13" s="120">
+      <c r="F13" s="119">
         <v>95</v>
       </c>
-      <c r="G13" s="119">
+      <c r="G13" s="118">
         <f t="shared" ref="G13" si="4">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C13-A13))*(D13/F13)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H13" s="119">
+      <c r="H13" s="118">
         <f t="shared" ref="H13" si="5">IFERROR(ROUND(MOD(A13+G13,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I13" s="120">
+      <c r="I13" s="119">
         <v>13</v>
       </c>
-      <c r="J13" s="119">
+      <c r="J13" s="118">
         <f t="shared" ref="J13" si="6">IFERROR(MOD(H13+I13,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K13" s="120">
+      <c r="K13" s="119">
         <v>2</v>
       </c>
       <c r="L13" s="29"/>
-      <c r="M13" s="122"/>
-      <c r="N13" s="119">
+      <c r="M13" s="116"/>
+      <c r="N13" s="118">
         <f>IFERROR(MOD(J13+K13,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O13" s="120">
+      <c r="O13" s="119">
         <v>11</v>
       </c>
       <c r="P13" s="42">
@@ -9789,23 +9789,23 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A14" s="120"/>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="120"/>
+      <c r="A14" s="119"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="119"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="123" t="s">
+      <c r="M14" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="119"/>
-      <c r="O14" s="120"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="119"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
       <c r="R14" s="45"/>
@@ -9813,49 +9813,49 @@
       <c r="T14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="131">
+      <c r="A15" s="117">
         <v>131</v>
       </c>
-      <c r="B15" s="131">
+      <c r="B15" s="117">
         <v>3500</v>
       </c>
-      <c r="C15" s="131">
+      <c r="C15" s="117">
         <v>215</v>
       </c>
-      <c r="D15" s="131">
+      <c r="D15" s="117">
         <v>17</v>
       </c>
-      <c r="E15" s="131">
+      <c r="E15" s="117">
         <v>-10</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="117">
         <v>95</v>
       </c>
-      <c r="G15" s="117">
+      <c r="G15" s="122">
         <f t="shared" ref="G15" si="8">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C15-A15))*(D15/F15)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H15" s="117">
+      <c r="H15" s="122">
         <f t="shared" ref="H15" si="9">IFERROR(ROUND(MOD(A15+G15,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I15" s="118">
+      <c r="I15" s="124">
         <v>13</v>
       </c>
-      <c r="J15" s="117">
+      <c r="J15" s="122">
         <f t="shared" ref="J15" si="10">IFERROR(MOD(H15+I15,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K15" s="118">
+      <c r="K15" s="124">
         <v>2</v>
       </c>
       <c r="L15" s="29"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="117">
+      <c r="M15" s="116"/>
+      <c r="N15" s="122">
         <f>IFERROR(MOD(J15+K15,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O15" s="118">
+      <c r="O15" s="124">
         <v>8</v>
       </c>
       <c r="P15" s="46">
@@ -9880,23 +9880,23 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A16" s="131"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="118"/>
+      <c r="A16" s="117"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="122"/>
+      <c r="H16" s="122"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="122"/>
+      <c r="K16" s="124"/>
       <c r="L16" s="29"/>
-      <c r="M16" s="123" t="s">
+      <c r="M16" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="117"/>
-      <c r="O16" s="118"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="124"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45"/>
@@ -9904,49 +9904,49 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A17" s="120">
+      <c r="A17" s="119">
         <v>131</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="119">
         <v>3500</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="119">
         <v>215</v>
       </c>
-      <c r="D17" s="120">
+      <c r="D17" s="119">
         <v>17</v>
       </c>
-      <c r="E17" s="120">
+      <c r="E17" s="119">
         <v>-10</v>
       </c>
-      <c r="F17" s="120">
+      <c r="F17" s="119">
         <v>95</v>
       </c>
-      <c r="G17" s="119">
+      <c r="G17" s="118">
         <f t="shared" ref="G17" si="12">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C17-A17))*(D17/F17)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H17" s="119">
+      <c r="H17" s="118">
         <f t="shared" ref="H17" si="13">IFERROR(ROUND(MOD(A17+G17,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I17" s="120">
+      <c r="I17" s="119">
         <v>13</v>
       </c>
-      <c r="J17" s="119">
+      <c r="J17" s="118">
         <f t="shared" ref="J17" si="14">IFERROR(MOD(H17+I17,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K17" s="120">
+      <c r="K17" s="119">
         <v>2</v>
       </c>
       <c r="L17" s="29"/>
-      <c r="M17" s="122"/>
-      <c r="N17" s="119">
+      <c r="M17" s="116"/>
+      <c r="N17" s="118">
         <f>IFERROR(MOD(J17+K17,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O17" s="120">
+      <c r="O17" s="119">
         <v>10</v>
       </c>
       <c r="P17" s="42">
@@ -9971,23 +9971,23 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A18" s="120"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
+      <c r="A18" s="119"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="119"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="123" t="s">
+      <c r="M18" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="119"/>
-      <c r="O18" s="120"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="119"/>
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
       <c r="R18" s="45"/>
@@ -9995,49 +9995,49 @@
       <c r="T18" s="44"/>
     </row>
     <row r="19" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="131">
+      <c r="A19" s="117">
         <v>131</v>
       </c>
-      <c r="B19" s="131">
+      <c r="B19" s="117">
         <v>3500</v>
       </c>
-      <c r="C19" s="131">
+      <c r="C19" s="117">
         <v>215</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="117">
         <v>17</v>
       </c>
-      <c r="E19" s="131">
+      <c r="E19" s="117">
         <v>-10</v>
       </c>
-      <c r="F19" s="131">
+      <c r="F19" s="117">
         <v>95</v>
       </c>
-      <c r="G19" s="117">
+      <c r="G19" s="122">
         <f t="shared" ref="G19" si="16">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C19-A19))*(D19/F19)))),0),"")</f>
         <v>10</v>
       </c>
-      <c r="H19" s="117">
+      <c r="H19" s="122">
         <f t="shared" ref="H19" si="17">IFERROR(ROUND(MOD(A19+G19,360),0),"")</f>
         <v>141</v>
       </c>
-      <c r="I19" s="118">
+      <c r="I19" s="124">
         <v>13</v>
       </c>
-      <c r="J19" s="117">
+      <c r="J19" s="122">
         <f t="shared" ref="J19" si="18">IFERROR(MOD(H19+I19,360),"")</f>
         <v>154</v>
       </c>
-      <c r="K19" s="118">
+      <c r="K19" s="124">
         <v>2</v>
       </c>
       <c r="L19" s="29"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="117">
+      <c r="M19" s="116"/>
+      <c r="N19" s="122">
         <f>IFERROR(MOD(J19+K19,360),"")</f>
         <v>156</v>
       </c>
-      <c r="O19" s="118">
+      <c r="O19" s="124">
         <v>11</v>
       </c>
       <c r="P19" s="46">
@@ -10062,23 +10062,23 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A20" s="131"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="118"/>
+      <c r="A20" s="117"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="122"/>
+      <c r="H20" s="122"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="122"/>
+      <c r="K20" s="124"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="123" t="s">
+      <c r="M20" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="N20" s="117"/>
-      <c r="O20" s="118"/>
+      <c r="N20" s="122"/>
+      <c r="O20" s="124"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="45"/>
@@ -10086,33 +10086,33 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A21" s="120"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="119" t="str">
+      <c r="A21" s="119"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="118" t="str">
         <f t="shared" ref="G21" si="20">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C21-A21))*(D21/F21)))),0),"")</f>
         <v/>
       </c>
-      <c r="H21" s="119" t="str">
+      <c r="H21" s="118" t="str">
         <f t="shared" ref="H21" si="21">IFERROR(ROUND(MOD(A21+G21,360),0),"")</f>
         <v/>
       </c>
-      <c r="I21" s="120"/>
-      <c r="J21" s="119" t="str">
+      <c r="I21" s="119"/>
+      <c r="J21" s="118" t="str">
         <f t="shared" ref="J21" si="22">IFERROR(MOD(H21+I21,360),"")</f>
         <v/>
       </c>
-      <c r="K21" s="120"/>
+      <c r="K21" s="119"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="119" t="str">
+      <c r="M21" s="116"/>
+      <c r="N21" s="118" t="str">
         <f>IFERROR(MOD(J21+K21,360),"")</f>
         <v/>
       </c>
-      <c r="O21" s="120"/>
+      <c r="O21" s="119"/>
       <c r="P21" s="42" t="str">
         <f>IFERROR(SQRT(F21^2+D21^2-2*F21*D21*COS(RADIANS(C21-A21-G21))),"")</f>
         <v/>
@@ -10135,21 +10135,21 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="119"/>
-      <c r="K22" s="120"/>
+      <c r="A22" s="119"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="119"/>
       <c r="L22" s="29"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="119"/>
-      <c r="O22" s="120"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="119"/>
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="45"/>
@@ -10157,33 +10157,33 @@
       <c r="T22" s="44"/>
     </row>
     <row r="23" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A23" s="131"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="117" t="str">
+      <c r="A23" s="117"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="122" t="str">
         <f t="shared" ref="G23" si="24">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C23-A23))*(D23/F23)))),0),"")</f>
         <v/>
       </c>
-      <c r="H23" s="117" t="str">
+      <c r="H23" s="122" t="str">
         <f t="shared" ref="H23" si="25">IFERROR(ROUND(MOD(A23+G23,360),0),"")</f>
         <v/>
       </c>
-      <c r="I23" s="118"/>
-      <c r="J23" s="117" t="str">
+      <c r="I23" s="124"/>
+      <c r="J23" s="122" t="str">
         <f t="shared" ref="J23" si="26">IFERROR(MOD(H23+I23,360),"")</f>
         <v/>
       </c>
-      <c r="K23" s="118"/>
+      <c r="K23" s="124"/>
       <c r="L23" s="29"/>
-      <c r="M23" s="122"/>
-      <c r="N23" s="117" t="str">
+      <c r="M23" s="116"/>
+      <c r="N23" s="122" t="str">
         <f>IFERROR(MOD(J23+K23,360),"")</f>
         <v/>
       </c>
-      <c r="O23" s="118"/>
+      <c r="O23" s="124"/>
       <c r="P23" s="46" t="str">
         <f>IFERROR(SQRT(F23^2+D23^2-2*F23*D23*COS(RADIANS(C23-A23-G23))),"")</f>
         <v/>
@@ -10206,21 +10206,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A24" s="131"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="118"/>
+      <c r="A24" s="117"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="124"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="118"/>
+      <c r="M24" s="115"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="124"/>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="45"/>
@@ -10228,33 +10228,33 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A25" s="120"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="119" t="str">
+      <c r="A25" s="119"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="118" t="str">
         <f t="shared" ref="G25" si="28">IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(C25-A25))*(D25/F25)))),0),"")</f>
         <v/>
       </c>
-      <c r="H25" s="119" t="str">
+      <c r="H25" s="118" t="str">
         <f t="shared" ref="H25" si="29">IFERROR(ROUND(MOD(A25+G25,360),0),"")</f>
         <v/>
       </c>
-      <c r="I25" s="120"/>
-      <c r="J25" s="119" t="str">
+      <c r="I25" s="119"/>
+      <c r="J25" s="118" t="str">
         <f t="shared" ref="J25" si="30">IFERROR(MOD(H25+I25,360),"")</f>
         <v/>
       </c>
-      <c r="K25" s="120"/>
+      <c r="K25" s="119"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="155"/>
-      <c r="N25" s="119" t="str">
+      <c r="M25" s="120"/>
+      <c r="N25" s="118" t="str">
         <f>IFERROR(MOD(J25+K25,360),"")</f>
         <v/>
       </c>
-      <c r="O25" s="120"/>
+      <c r="O25" s="119"/>
       <c r="P25" s="42" t="str">
         <f>IFERROR(SQRT(F25^2+D25^2-2*F25*D25*COS(RADIANS(C25-A25-G25))),"")</f>
         <v/>
@@ -10277,23 +10277,23 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A26" s="120"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="119"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="120"/>
+      <c r="A26" s="119"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="119"/>
       <c r="L26" s="29"/>
       <c r="M26" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N26" s="119"/>
-      <c r="O26" s="120"/>
+      <c r="N26" s="118"/>
+      <c r="O26" s="119"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
       <c r="R26" s="45"/>
@@ -10301,19 +10301,19 @@
       <c r="T26" s="44"/>
     </row>
     <row r="27" spans="1:20" ht="25.5" thickBot="1">
-      <c r="A27" s="137" t="s">
+      <c r="A27" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
-      <c r="J27" s="138"/>
-      <c r="K27" s="139"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="99"/>
       <c r="L27" s="30"/>
       <c r="M27" s="31" t="s">
         <v>67</v>
@@ -10336,23 +10336,143 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A28" s="140"/>
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="141"/>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="142"/>
+      <c r="A28" s="100"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="102"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="144">
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="A27:K28"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="O11:O12"/>
@@ -10377,126 +10497,6 @@
     <mergeCell ref="Q3:R4"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A27:K28"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="G1:I2"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:O4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -10508,7 +10508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CFACEB-C7F9-4EC2-B331-5938690C3313}">
   <dimension ref="B1:V46"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10524,18 +10526,18 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:22" ht="20.25" thickBot="1">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="188" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
-      <c r="I2" s="179"/>
-      <c r="J2" s="180"/>
-      <c r="L2" s="186" t="s">
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="190"/>
+      <c r="L2" s="93" t="s">
         <v>98</v>
       </c>
     </row>
@@ -10549,19 +10551,19 @@
       <c r="H3" s="67"/>
       <c r="I3" s="67"/>
       <c r="J3" s="68"/>
-      <c r="L3" s="187" t="s">
+      <c r="L3" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="188"/>
-      <c r="N3" s="188"/>
-      <c r="O3" s="188"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="188"/>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="189"/>
+      <c r="M3" s="196"/>
+      <c r="N3" s="196"/>
+      <c r="O3" s="196"/>
+      <c r="P3" s="196"/>
+      <c r="Q3" s="196"/>
+      <c r="R3" s="196"/>
+      <c r="S3" s="196"/>
+      <c r="T3" s="196"/>
+      <c r="U3" s="196"/>
+      <c r="V3" s="197"/>
     </row>
     <row r="4" spans="2:22" ht="18.75">
       <c r="B4" s="66"/>
@@ -10584,17 +10586,17 @@
       </c>
       <c r="I4" s="69"/>
       <c r="J4" s="68"/>
-      <c r="L4" s="190"/>
-      <c r="M4" s="191"/>
-      <c r="N4" s="191"/>
-      <c r="O4" s="191"/>
-      <c r="P4" s="191"/>
-      <c r="Q4" s="191"/>
-      <c r="R4" s="191"/>
-      <c r="S4" s="191"/>
-      <c r="T4" s="191"/>
-      <c r="U4" s="191"/>
-      <c r="V4" s="192"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="199"/>
+      <c r="N4" s="199"/>
+      <c r="O4" s="199"/>
+      <c r="P4" s="199"/>
+      <c r="Q4" s="199"/>
+      <c r="R4" s="199"/>
+      <c r="S4" s="199"/>
+      <c r="T4" s="199"/>
+      <c r="U4" s="199"/>
+      <c r="V4" s="200"/>
     </row>
     <row r="5" spans="2:22" ht="18.75">
       <c r="B5" s="66"/>
@@ -10617,17 +10619,17 @@
       </c>
       <c r="I5" s="69"/>
       <c r="J5" s="68"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="191"/>
-      <c r="P5" s="191"/>
-      <c r="Q5" s="191"/>
-      <c r="R5" s="191"/>
-      <c r="S5" s="191"/>
-      <c r="T5" s="191"/>
-      <c r="U5" s="191"/>
-      <c r="V5" s="192"/>
+      <c r="L5" s="198"/>
+      <c r="M5" s="199"/>
+      <c r="N5" s="199"/>
+      <c r="O5" s="199"/>
+      <c r="P5" s="199"/>
+      <c r="Q5" s="199"/>
+      <c r="R5" s="199"/>
+      <c r="S5" s="199"/>
+      <c r="T5" s="199"/>
+      <c r="U5" s="199"/>
+      <c r="V5" s="200"/>
     </row>
     <row r="6" spans="2:22" ht="18.75">
       <c r="B6" s="66"/>
@@ -10643,17 +10645,17 @@
       <c r="H6" s="69"/>
       <c r="I6" s="69"/>
       <c r="J6" s="68"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="191"/>
-      <c r="N6" s="191"/>
-      <c r="O6" s="191"/>
-      <c r="P6" s="191"/>
-      <c r="Q6" s="191"/>
-      <c r="R6" s="191"/>
-      <c r="S6" s="191"/>
-      <c r="T6" s="191"/>
-      <c r="U6" s="191"/>
-      <c r="V6" s="192"/>
+      <c r="L6" s="198"/>
+      <c r="M6" s="199"/>
+      <c r="N6" s="199"/>
+      <c r="O6" s="199"/>
+      <c r="P6" s="199"/>
+      <c r="Q6" s="199"/>
+      <c r="R6" s="199"/>
+      <c r="S6" s="199"/>
+      <c r="T6" s="199"/>
+      <c r="U6" s="199"/>
+      <c r="V6" s="200"/>
     </row>
     <row r="7" spans="2:22" ht="18.75">
       <c r="B7" s="66"/>
@@ -10676,17 +10678,17 @@
       </c>
       <c r="I7" s="69"/>
       <c r="J7" s="68"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="191"/>
-      <c r="N7" s="191"/>
-      <c r="O7" s="191"/>
-      <c r="P7" s="191"/>
-      <c r="Q7" s="191"/>
-      <c r="R7" s="191"/>
-      <c r="S7" s="191"/>
-      <c r="T7" s="191"/>
-      <c r="U7" s="191"/>
-      <c r="V7" s="192"/>
+      <c r="L7" s="198"/>
+      <c r="M7" s="199"/>
+      <c r="N7" s="199"/>
+      <c r="O7" s="199"/>
+      <c r="P7" s="199"/>
+      <c r="Q7" s="199"/>
+      <c r="R7" s="199"/>
+      <c r="S7" s="199"/>
+      <c r="T7" s="199"/>
+      <c r="U7" s="199"/>
+      <c r="V7" s="200"/>
     </row>
     <row r="8" spans="2:22">
       <c r="B8" s="66"/>
@@ -10705,17 +10707,17 @@
       </c>
       <c r="I8" s="69"/>
       <c r="J8" s="68"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="191"/>
-      <c r="N8" s="191"/>
-      <c r="O8" s="191"/>
-      <c r="P8" s="191"/>
-      <c r="Q8" s="191"/>
-      <c r="R8" s="191"/>
-      <c r="S8" s="191"/>
-      <c r="T8" s="191"/>
-      <c r="U8" s="191"/>
-      <c r="V8" s="192"/>
+      <c r="L8" s="198"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="199"/>
+      <c r="R8" s="199"/>
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="200"/>
     </row>
     <row r="9" spans="2:22">
       <c r="B9" s="66"/>
@@ -10727,66 +10729,66 @@
       <c r="H9" s="67"/>
       <c r="I9" s="67"/>
       <c r="J9" s="68"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="191"/>
-      <c r="N9" s="191"/>
-      <c r="O9" s="191"/>
-      <c r="P9" s="191"/>
-      <c r="Q9" s="191"/>
-      <c r="R9" s="191"/>
-      <c r="S9" s="191"/>
-      <c r="T9" s="191"/>
-      <c r="U9" s="191"/>
-      <c r="V9" s="192"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="199"/>
+      <c r="N9" s="199"/>
+      <c r="O9" s="199"/>
+      <c r="P9" s="199"/>
+      <c r="Q9" s="199"/>
+      <c r="R9" s="199"/>
+      <c r="S9" s="199"/>
+      <c r="T9" s="199"/>
+      <c r="U9" s="199"/>
+      <c r="V9" s="200"/>
     </row>
     <row r="10" spans="2:22" ht="18.75">
       <c r="B10" s="66"/>
-      <c r="C10" s="185" t="s">
+      <c r="C10" s="195" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="185"/>
+      <c r="D10" s="195"/>
       <c r="E10" s="67"/>
       <c r="F10" s="67"/>
       <c r="G10" s="67"/>
       <c r="H10" s="67"/>
       <c r="I10" s="67"/>
       <c r="J10" s="68"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="191"/>
-      <c r="N10" s="191"/>
-      <c r="O10" s="191"/>
-      <c r="P10" s="191"/>
-      <c r="Q10" s="191"/>
-      <c r="R10" s="191"/>
-      <c r="S10" s="191"/>
-      <c r="T10" s="191"/>
-      <c r="U10" s="191"/>
-      <c r="V10" s="192"/>
+      <c r="L10" s="198"/>
+      <c r="M10" s="199"/>
+      <c r="N10" s="199"/>
+      <c r="O10" s="199"/>
+      <c r="P10" s="199"/>
+      <c r="Q10" s="199"/>
+      <c r="R10" s="199"/>
+      <c r="S10" s="199"/>
+      <c r="T10" s="199"/>
+      <c r="U10" s="199"/>
+      <c r="V10" s="200"/>
     </row>
     <row r="11" spans="2:22" ht="19.5" thickBot="1">
       <c r="B11" s="66"/>
-      <c r="C11" s="184">
+      <c r="C11" s="194">
         <f>IFERROR(ROUND(DEGREES(ASIN((SIN(RADIANS(Wd-HEading))*(Ws/TrueAirSpeed)))),0),"")</f>
         <v>9</v>
       </c>
-      <c r="D11" s="184"/>
+      <c r="D11" s="194"/>
       <c r="E11" s="67"/>
       <c r="F11" s="67"/>
       <c r="G11" s="67"/>
       <c r="H11" s="67"/>
       <c r="I11" s="67"/>
       <c r="J11" s="68"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="194"/>
-      <c r="N11" s="194"/>
-      <c r="O11" s="194"/>
-      <c r="P11" s="194"/>
-      <c r="Q11" s="194"/>
-      <c r="R11" s="194"/>
-      <c r="S11" s="194"/>
-      <c r="T11" s="194"/>
-      <c r="U11" s="194"/>
-      <c r="V11" s="195"/>
+      <c r="L11" s="201"/>
+      <c r="M11" s="202"/>
+      <c r="N11" s="202"/>
+      <c r="O11" s="202"/>
+      <c r="P11" s="202"/>
+      <c r="Q11" s="202"/>
+      <c r="R11" s="202"/>
+      <c r="S11" s="202"/>
+      <c r="T11" s="202"/>
+      <c r="U11" s="202"/>
+      <c r="V11" s="203"/>
     </row>
     <row r="12" spans="2:22">
       <c r="B12" s="66"/>
@@ -10844,17 +10846,17 @@
       <c r="J16" s="68"/>
     </row>
     <row r="17" spans="2:22" ht="19.5">
-      <c r="B17" s="181" t="s">
+      <c r="B17" s="191" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="182"/>
-      <c r="D17" s="182"/>
-      <c r="E17" s="182"/>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182"/>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
-      <c r="J17" s="183"/>
+      <c r="C17" s="192"/>
+      <c r="D17" s="192"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="2:22" ht="15.75" thickBot="1">
       <c r="B18" s="66"/>
@@ -10888,8 +10890,8 @@
       </c>
       <c r="I19" s="67"/>
       <c r="J19" s="68"/>
-      <c r="L19" s="186" t="s">
-        <v>101</v>
+      <c r="L19" s="93" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:22" ht="19.5" customHeight="1" thickBot="1">
@@ -10909,19 +10911,19 @@
       </c>
       <c r="I20" s="67"/>
       <c r="J20" s="68"/>
-      <c r="L20" s="187" t="s">
-        <v>100</v>
-      </c>
-      <c r="M20" s="196"/>
-      <c r="N20" s="196"/>
-      <c r="O20" s="196"/>
-      <c r="P20" s="196"/>
-      <c r="Q20" s="196"/>
-      <c r="R20" s="196"/>
-      <c r="S20" s="196"/>
-      <c r="T20" s="196"/>
-      <c r="U20" s="196"/>
-      <c r="V20" s="197"/>
+      <c r="L20" s="179" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" s="180"/>
+      <c r="N20" s="180"/>
+      <c r="O20" s="180"/>
+      <c r="P20" s="180"/>
+      <c r="Q20" s="180"/>
+      <c r="R20" s="180"/>
+      <c r="S20" s="180"/>
+      <c r="T20" s="180"/>
+      <c r="U20" s="180"/>
+      <c r="V20" s="181"/>
     </row>
     <row r="21" spans="2:22">
       <c r="B21" s="66"/>
@@ -10935,17 +10937,17 @@
       <c r="H21" s="67"/>
       <c r="I21" s="67"/>
       <c r="J21" s="68"/>
-      <c r="L21" s="198"/>
-      <c r="M21" s="199"/>
-      <c r="N21" s="199"/>
-      <c r="O21" s="199"/>
-      <c r="P21" s="199"/>
-      <c r="Q21" s="199"/>
-      <c r="R21" s="199"/>
-      <c r="S21" s="199"/>
-      <c r="T21" s="199"/>
-      <c r="U21" s="199"/>
-      <c r="V21" s="200"/>
+      <c r="L21" s="182"/>
+      <c r="M21" s="183"/>
+      <c r="N21" s="183"/>
+      <c r="O21" s="183"/>
+      <c r="P21" s="183"/>
+      <c r="Q21" s="183"/>
+      <c r="R21" s="183"/>
+      <c r="S21" s="183"/>
+      <c r="T21" s="183"/>
+      <c r="U21" s="183"/>
+      <c r="V21" s="184"/>
     </row>
     <row r="22" spans="2:22">
       <c r="B22" s="66"/>
@@ -10957,17 +10959,17 @@
       <c r="H22" s="67"/>
       <c r="I22" s="67"/>
       <c r="J22" s="68"/>
-      <c r="L22" s="198"/>
-      <c r="M22" s="199"/>
-      <c r="N22" s="199"/>
-      <c r="O22" s="199"/>
-      <c r="P22" s="199"/>
-      <c r="Q22" s="199"/>
-      <c r="R22" s="199"/>
-      <c r="S22" s="199"/>
-      <c r="T22" s="199"/>
-      <c r="U22" s="199"/>
-      <c r="V22" s="200"/>
+      <c r="L22" s="182"/>
+      <c r="M22" s="183"/>
+      <c r="N22" s="183"/>
+      <c r="O22" s="183"/>
+      <c r="P22" s="183"/>
+      <c r="Q22" s="183"/>
+      <c r="R22" s="183"/>
+      <c r="S22" s="183"/>
+      <c r="T22" s="183"/>
+      <c r="U22" s="183"/>
+      <c r="V22" s="184"/>
     </row>
     <row r="23" spans="2:22">
       <c r="B23" s="66"/>
@@ -10987,17 +10989,17 @@
       <c r="H23" s="67"/>
       <c r="I23" s="67"/>
       <c r="J23" s="68"/>
-      <c r="L23" s="198"/>
-      <c r="M23" s="199"/>
-      <c r="N23" s="199"/>
-      <c r="O23" s="199"/>
-      <c r="P23" s="199"/>
-      <c r="Q23" s="199"/>
-      <c r="R23" s="199"/>
-      <c r="S23" s="199"/>
-      <c r="T23" s="199"/>
-      <c r="U23" s="199"/>
-      <c r="V23" s="200"/>
+      <c r="L23" s="182"/>
+      <c r="M23" s="183"/>
+      <c r="N23" s="183"/>
+      <c r="O23" s="183"/>
+      <c r="P23" s="183"/>
+      <c r="Q23" s="183"/>
+      <c r="R23" s="183"/>
+      <c r="S23" s="183"/>
+      <c r="T23" s="183"/>
+      <c r="U23" s="183"/>
+      <c r="V23" s="184"/>
     </row>
     <row r="24" spans="2:22">
       <c r="B24" s="66"/>
@@ -11017,17 +11019,17 @@
       <c r="H24" s="67"/>
       <c r="I24" s="67"/>
       <c r="J24" s="68"/>
-      <c r="L24" s="198"/>
-      <c r="M24" s="199"/>
-      <c r="N24" s="199"/>
-      <c r="O24" s="199"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="199"/>
-      <c r="R24" s="199"/>
-      <c r="S24" s="199"/>
-      <c r="T24" s="199"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="200"/>
+      <c r="L24" s="182"/>
+      <c r="M24" s="183"/>
+      <c r="N24" s="183"/>
+      <c r="O24" s="183"/>
+      <c r="P24" s="183"/>
+      <c r="Q24" s="183"/>
+      <c r="R24" s="183"/>
+      <c r="S24" s="183"/>
+      <c r="T24" s="183"/>
+      <c r="U24" s="183"/>
+      <c r="V24" s="184"/>
     </row>
     <row r="25" spans="2:22">
       <c r="B25" s="66"/>
@@ -11039,17 +11041,17 @@
       <c r="H25" s="67"/>
       <c r="I25" s="67"/>
       <c r="J25" s="68"/>
-      <c r="L25" s="198"/>
-      <c r="M25" s="199"/>
-      <c r="N25" s="199"/>
-      <c r="O25" s="199"/>
-      <c r="P25" s="199"/>
-      <c r="Q25" s="199"/>
-      <c r="R25" s="199"/>
-      <c r="S25" s="199"/>
-      <c r="T25" s="199"/>
-      <c r="U25" s="199"/>
-      <c r="V25" s="200"/>
+      <c r="L25" s="182"/>
+      <c r="M25" s="183"/>
+      <c r="N25" s="183"/>
+      <c r="O25" s="183"/>
+      <c r="P25" s="183"/>
+      <c r="Q25" s="183"/>
+      <c r="R25" s="183"/>
+      <c r="S25" s="183"/>
+      <c r="T25" s="183"/>
+      <c r="U25" s="183"/>
+      <c r="V25" s="184"/>
     </row>
     <row r="26" spans="2:22">
       <c r="B26" s="66"/>
@@ -11061,17 +11063,17 @@
       <c r="H26" s="67"/>
       <c r="I26" s="67"/>
       <c r="J26" s="68"/>
-      <c r="L26" s="198"/>
-      <c r="M26" s="199"/>
-      <c r="N26" s="199"/>
-      <c r="O26" s="199"/>
-      <c r="P26" s="199"/>
-      <c r="Q26" s="199"/>
-      <c r="R26" s="199"/>
-      <c r="S26" s="199"/>
-      <c r="T26" s="199"/>
-      <c r="U26" s="199"/>
-      <c r="V26" s="200"/>
+      <c r="L26" s="182"/>
+      <c r="M26" s="183"/>
+      <c r="N26" s="183"/>
+      <c r="O26" s="183"/>
+      <c r="P26" s="183"/>
+      <c r="Q26" s="183"/>
+      <c r="R26" s="183"/>
+      <c r="S26" s="183"/>
+      <c r="T26" s="183"/>
+      <c r="U26" s="183"/>
+      <c r="V26" s="184"/>
     </row>
     <row r="27" spans="2:22">
       <c r="B27" s="66"/>
@@ -11083,17 +11085,17 @@
       <c r="H27" s="67"/>
       <c r="I27" s="67"/>
       <c r="J27" s="68"/>
-      <c r="L27" s="198"/>
-      <c r="M27" s="199"/>
-      <c r="N27" s="199"/>
-      <c r="O27" s="199"/>
-      <c r="P27" s="199"/>
-      <c r="Q27" s="199"/>
-      <c r="R27" s="199"/>
-      <c r="S27" s="199"/>
-      <c r="T27" s="199"/>
-      <c r="U27" s="199"/>
-      <c r="V27" s="200"/>
+      <c r="L27" s="182"/>
+      <c r="M27" s="183"/>
+      <c r="N27" s="183"/>
+      <c r="O27" s="183"/>
+      <c r="P27" s="183"/>
+      <c r="Q27" s="183"/>
+      <c r="R27" s="183"/>
+      <c r="S27" s="183"/>
+      <c r="T27" s="183"/>
+      <c r="U27" s="183"/>
+      <c r="V27" s="184"/>
     </row>
     <row r="28" spans="2:22">
       <c r="B28" s="66"/>
@@ -11105,17 +11107,17 @@
       <c r="H28" s="67"/>
       <c r="I28" s="67"/>
       <c r="J28" s="68"/>
-      <c r="L28" s="198"/>
-      <c r="M28" s="199"/>
-      <c r="N28" s="199"/>
-      <c r="O28" s="199"/>
-      <c r="P28" s="199"/>
-      <c r="Q28" s="199"/>
-      <c r="R28" s="199"/>
-      <c r="S28" s="199"/>
-      <c r="T28" s="199"/>
-      <c r="U28" s="199"/>
-      <c r="V28" s="200"/>
+      <c r="L28" s="182"/>
+      <c r="M28" s="183"/>
+      <c r="N28" s="183"/>
+      <c r="O28" s="183"/>
+      <c r="P28" s="183"/>
+      <c r="Q28" s="183"/>
+      <c r="R28" s="183"/>
+      <c r="S28" s="183"/>
+      <c r="T28" s="183"/>
+      <c r="U28" s="183"/>
+      <c r="V28" s="184"/>
     </row>
     <row r="29" spans="2:22">
       <c r="B29" s="66"/>
@@ -11127,17 +11129,17 @@
       <c r="H29" s="67"/>
       <c r="I29" s="67"/>
       <c r="J29" s="68"/>
-      <c r="L29" s="198"/>
-      <c r="M29" s="199"/>
-      <c r="N29" s="199"/>
-      <c r="O29" s="199"/>
-      <c r="P29" s="199"/>
-      <c r="Q29" s="199"/>
-      <c r="R29" s="199"/>
-      <c r="S29" s="199"/>
-      <c r="T29" s="199"/>
-      <c r="U29" s="199"/>
-      <c r="V29" s="200"/>
+      <c r="L29" s="182"/>
+      <c r="M29" s="183"/>
+      <c r="N29" s="183"/>
+      <c r="O29" s="183"/>
+      <c r="P29" s="183"/>
+      <c r="Q29" s="183"/>
+      <c r="R29" s="183"/>
+      <c r="S29" s="183"/>
+      <c r="T29" s="183"/>
+      <c r="U29" s="183"/>
+      <c r="V29" s="184"/>
     </row>
     <row r="30" spans="2:22">
       <c r="B30" s="66"/>
@@ -11149,17 +11151,17 @@
       <c r="H30" s="67"/>
       <c r="I30" s="67"/>
       <c r="J30" s="68"/>
-      <c r="L30" s="198"/>
-      <c r="M30" s="199"/>
-      <c r="N30" s="199"/>
-      <c r="O30" s="199"/>
-      <c r="P30" s="199"/>
-      <c r="Q30" s="199"/>
-      <c r="R30" s="199"/>
-      <c r="S30" s="199"/>
-      <c r="T30" s="199"/>
-      <c r="U30" s="199"/>
-      <c r="V30" s="200"/>
+      <c r="L30" s="182"/>
+      <c r="M30" s="183"/>
+      <c r="N30" s="183"/>
+      <c r="O30" s="183"/>
+      <c r="P30" s="183"/>
+      <c r="Q30" s="183"/>
+      <c r="R30" s="183"/>
+      <c r="S30" s="183"/>
+      <c r="T30" s="183"/>
+      <c r="U30" s="183"/>
+      <c r="V30" s="184"/>
     </row>
     <row r="31" spans="2:22" ht="15.75" thickBot="1">
       <c r="B31" s="66"/>
@@ -11171,17 +11173,17 @@
       <c r="H31" s="67"/>
       <c r="I31" s="67"/>
       <c r="J31" s="68"/>
-      <c r="L31" s="201"/>
-      <c r="M31" s="202"/>
-      <c r="N31" s="202"/>
-      <c r="O31" s="202"/>
-      <c r="P31" s="202"/>
-      <c r="Q31" s="202"/>
-      <c r="R31" s="202"/>
-      <c r="S31" s="202"/>
-      <c r="T31" s="202"/>
-      <c r="U31" s="202"/>
-      <c r="V31" s="203"/>
+      <c r="L31" s="185"/>
+      <c r="M31" s="186"/>
+      <c r="N31" s="186"/>
+      <c r="O31" s="186"/>
+      <c r="P31" s="186"/>
+      <c r="Q31" s="186"/>
+      <c r="R31" s="186"/>
+      <c r="S31" s="186"/>
+      <c r="T31" s="186"/>
+      <c r="U31" s="186"/>
+      <c r="V31" s="187"/>
     </row>
     <row r="32" spans="2:22">
       <c r="B32" s="66"/>

</xml_diff>